<commit_message>
modified index to replace OUTCOMES with MS
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\DP3-MS-SLE\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599E9CF6-4DBE-496C-8721-E96912B73C72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8376157-47EC-43AA-A5D6-4F24C838F7D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="9045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="129">
   <si>
     <t>release</t>
   </si>
@@ -175,158 +175,13 @@
     <t>03_T2_22_create_components_SLE</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>D3_algorithms_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-  </si>
-  <si>
     <t>just the dates when persons turn positive for each algorithm if any</t>
   </si>
   <si>
     <t>03_T2_30_create_algorithms</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>D3_components_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>_SAP1 D3_components_multiple_lookback_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> D3_study_population_SAP1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>D3_algorithms_multiple_lookback_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-  </si>
-  <si>
     <t>only for women in the study at 31 december 2019 and in the population since 5 or 10 years: all 5 algorithms calculated with multiple look back periods</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>D3_components_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>_SAP1 D3_components_multiple_lookback_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> D3_study_population_SAP1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>D4_prevalence_period_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
   </si>
   <si>
     <t>aggregated prevalence of all the MS algorithms computed with methods 'period prevalence'</t>
@@ -335,56 +190,7 @@
     <t>03_T3_40_compute_period_prevalence_MS</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>D3_algorithms_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> D3_study_population_SAP1</t>
-    </r>
-  </si>
-  <si>
-    <t>D4_prevalence_period_OUTCOME_summary_levels</t>
-  </si>
-  <si>
     <t>g_export</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>D4_prevalence_persontime_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
   </si>
   <si>
     <t>Yearly prevalence of all the MS algorithms computed with methods 'persontime prevalence'</t>
@@ -393,198 +199,13 @@
     <t>03_T3_41_compute_persontime_prevalence_MS</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>D3_algorithms_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> D3_study_population_SAP1</t>
-    </r>
-  </si>
-  <si>
-    <t>D4_prevalence_persontime_OUTCOME_summary_level</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>D4_prevalence_average_point_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-  </si>
-  <si>
     <t>montly aggregated prevalence of all the MS algorithms computed with methods 'point prevalence'</t>
   </si>
   <si>
     <t>03_T3_42_compute_monthly_point_prevalence_MS</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>D3_algorithms_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> D3_study_population_SAP1</t>
-    </r>
-  </si>
-  <si>
-    <t>D4_prevalence_average_point_OUTCOME_summary_levels</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>D4_prevalence_aggregated_multiple_lookback_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-  </si>
-  <si>
-    <t>aggregate D3_algorithms_multiple_lookback_OUTCOME per dimensions</t>
-  </si>
-  <si>
     <t>03_T3_50_point_prevalence_multiple_lookback</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>D3_algorithms_multiple_lookback_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>D4_prevalence_aggregated_multiple_lookback_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>summary_level</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>D3_algorithms_multiple_lookback_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>D5_N_women_and_ranges_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
   </si>
   <si>
     <t>values needed for Template 1 of the SAP: for each component N of women median time in study population and IQR (Years) and median and IQR age at time of first criteria</t>
@@ -593,117 +214,7 @@
     <t>04_T4_10_create_N_women_and_ranges_MS</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>D3_components_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>_SAP1 D3_study_population_SAP1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>D5_N_women_and_ranges_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>_masked</t>
-    </r>
-  </si>
-  <si>
-    <t>D5_N_women_and_ranges_OUTCOME with masked counts</t>
-  </si>
-  <si>
     <t>05_T5_10_censor_small_count</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Flowchart_exclusion_criteria D5_meaning_occurences D4_prevalence_aggregated_all_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> D4_prevalence_aggregated_multiple_lookback_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> D5_N_women_and_ranges_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
   </si>
   <si>
     <t>Flowchart_exclusion_criteria_masked</t>
@@ -712,182 +223,19 @@
     <t>Flowchart_exclusion_criteria with masked counts</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Flowchart_exclusion_criteria D5_meaning_occurences D4_prevalence_aggregated_all_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> D4_prevalence_aggregated_multiple_lookback_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> D5_N_women_and_ranges_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-  </si>
-  <si>
     <t>D5_meaning_occurences_masked</t>
   </si>
   <si>
     <t>D5_meaning_occurences with masked counts</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Flowchart_exclusion_criteria D5_meaning_occurences D4_prevalence_aggregated_all_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> D4_prevalence_aggregated_multiple_lookback_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> D5_N_women_and_ranges_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-  </si>
-  <si>
     <t>not included yet</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>D4_prevalence_aggregated_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>selected</t>
-    </r>
   </si>
   <si>
     <t>apply the Cube format to aggregated prevalence of all the MS algorithms in all the study periods and with all the methods</t>
   </si>
   <si>
     <t>06_T3_10_remove_small_counts</t>
-  </si>
-  <si>
-    <t>D4_prevalence_aggregated_all_OUTCOME D4_prevalence_aggregated_multiple_lookback_OUTCOME</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>D4_prevalence_aggregated_multiple_lookback_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>_selected</t>
-    </r>
   </si>
   <si>
     <t>D3_SAP1_MS-COHORT</t>
@@ -992,8 +340,11 @@
     <t>slug</t>
   </si>
   <si>
+    <t>08_T4_30_create_prevalence_MS_in_pregnancy_cohort</t>
+  </si>
+  <si>
     <r>
-      <t>D3_components_</t>
+      <t>D3_algorithms_</t>
     </r>
     <r>
       <rPr>
@@ -1002,40 +353,78 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>OUTCOME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>_SAP1</t>
+      <t>MS</t>
     </r>
   </si>
   <si>
-    <r>
-      <t>D3_components_multiple_lookback_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
+    <t>D3_components_MS_SAP1</t>
   </si>
   <si>
-    <t>08_T4_30_create_prevalence_MS_in_pregnancy_cohort</t>
+    <t>D3_components_multiple_lookback_MS</t>
+  </si>
+  <si>
+    <t>D3_components_MS_SAP1 D3_components_multiple_lookback_MS D3_study_population_SAP1</t>
+  </si>
+  <si>
+    <t>D3_algorithms_multiple_lookback_MS</t>
+  </si>
+  <si>
+    <t>D4_prevalence_period_MS</t>
+  </si>
+  <si>
+    <t>D4_prevalence_period_MS_summary_levels</t>
+  </si>
+  <si>
+    <t>D4_prevalence_persontime_MS</t>
+  </si>
+  <si>
+    <t>D4_prevalence_persontime_MS_summary_level</t>
+  </si>
+  <si>
+    <t>D4_prevalence_average_point_MS</t>
+  </si>
+  <si>
+    <t>D4_prevalence_average_point_MS_summary_levels</t>
+  </si>
+  <si>
+    <t>D4_prevalence_aggregated_multiple_lookback_MS</t>
+  </si>
+  <si>
+    <t>aggregate D3_algorithms_multiple_lookback_MS per dimensions</t>
+  </si>
+  <si>
+    <t>D4_prevalence_aggregated_multiple_lookback_MS_summary_level</t>
+  </si>
+  <si>
+    <t>D5_N_women_and_ranges_MS</t>
+  </si>
+  <si>
+    <t>D3_components_MS_SAP1 D3_study_population_SAP1</t>
+  </si>
+  <si>
+    <t>D5_N_women_and_ranges_MS_masked</t>
+  </si>
+  <si>
+    <t>D5_N_women_and_ranges_MS with masked counts</t>
+  </si>
+  <si>
+    <t>Flowchart_exclusion_criteria D5_meaning_occurences D4_prevalence_aggregated_all_MS D4_prevalence_aggregated_multiple_lookback_MS D5_N_women_and_ranges_MS</t>
+  </si>
+  <si>
+    <t>D4_prevalence_aggregated_MS_selected</t>
+  </si>
+  <si>
+    <t>D4_prevalence_aggregated_all_MS D4_prevalence_aggregated_multiple_lookback_MS</t>
+  </si>
+  <si>
+    <t>D4_prevalence_aggregated_multiple_lookback_MS_selected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1079,23 +468,6 @@
       <sz val="9"/>
       <color rgb="FF1F1F1F"/>
       <name val="&quot;Google Sans&quot;"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1234,12 +606,12 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1461,10 +833,10 @@
   <dimension ref="A1:AA1025"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1507,7 +879,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -2004,7 +1376,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="7" t="s">
@@ -2043,7 +1415,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="7" t="s">
@@ -2082,16 +1454,16 @@
         <v>9</v>
       </c>
       <c r="B16" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="D16" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="E16" s="14" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="9" t="s">
@@ -2123,16 +1495,16 @@
         <v>9</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="9" t="s">
@@ -2164,16 +1536,16 @@
         <v>9</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="9" t="s">
@@ -2205,16 +1577,16 @@
         <v>9</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="4"/>
       <c r="G19" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="3"/>
@@ -2242,16 +1614,16 @@
         <v>9</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="9" t="s">
@@ -2283,16 +1655,16 @@
         <v>9</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>68</v>
+        <v>115</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="4"/>
       <c r="G21" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="3"/>
@@ -2320,16 +1692,16 @@
         <v>9</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="9" t="s">
@@ -2361,16 +1733,16 @@
         <v>9</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E23" s="15"/>
       <c r="F23" s="4"/>
       <c r="G23" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="3"/>
@@ -2398,16 +1770,16 @@
         <v>9</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="9" t="s">
@@ -2439,20 +1811,20 @@
         <v>9</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="4"/>
@@ -2480,16 +1852,16 @@
         <v>9</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="9" t="s">
@@ -2521,20 +1893,20 @@
         <v>9</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="4"/>
@@ -2562,20 +1934,20 @@
         <v>9</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="4"/>
@@ -2603,20 +1975,20 @@
         <v>9</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="4"/>
@@ -2641,19 +2013,19 @@
     </row>
     <row r="30" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="9"/>
@@ -2680,19 +2052,19 @@
     </row>
     <row r="31" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B31" s="39" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="9"/>
@@ -2719,19 +2091,19 @@
     </row>
     <row r="32" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -2758,25 +2130,25 @@
     </row>
     <row r="33" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="F33" s="30"/>
       <c r="G33" s="4"/>
       <c r="H33" s="6"/>
       <c r="I33" s="3" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -2799,25 +2171,25 @@
     </row>
     <row r="34" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="D34" s="28" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="F34" s="30"/>
       <c r="G34" s="4"/>
       <c r="H34" s="6"/>
       <c r="I34" s="3" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -2840,25 +2212,25 @@
     </row>
     <row r="35" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="D35" s="28" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="F35" s="30"/>
       <c r="G35" s="4"/>
       <c r="H35" s="6"/>
       <c r="I35" s="3" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -2881,25 +2253,25 @@
     </row>
     <row r="36" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="6"/>
       <c r="I36" s="3" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -2922,19 +2294,19 @@
     </row>
     <row r="37" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -2961,25 +2333,25 @@
     </row>
     <row r="38" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>122</v>
-      </c>
       <c r="D38" s="3" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="6"/>
       <c r="I38" s="3" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -3002,25 +2374,25 @@
     </row>
     <row r="39" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="D39" s="32" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="E39" s="33" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="F39" s="34"/>
       <c r="G39" s="4"/>
       <c r="H39" s="6"/>
       <c r="I39" s="3" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -3043,21 +2415,21 @@
     </row>
     <row r="40" spans="1:27" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="E40" s="25"/>
       <c r="F40" s="4"/>
       <c r="G40" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="3"/>
@@ -3082,25 +2454,25 @@
     </row>
     <row r="41" spans="1:27" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="E41" s="25" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="6"/>
       <c r="I41" s="3" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -3123,25 +2495,25 @@
     </row>
     <row r="42" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="E42" s="25" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
       <c r="H42" s="6"/>
       <c r="I42" s="3" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>

</xml_diff>

<commit_message>
follow up to previous commit
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="130">
   <si>
     <t>release</t>
   </si>
@@ -243,9 +243,6 @@
     <t>contains the cohort of study population who have MS based on the algorithm chosen at the end of SAP1</t>
   </si>
   <si>
-    <t>07_T3_10_create_MS-COHORT</t>
-  </si>
-  <si>
     <t>D3_algorithms_MS D3_study_population_SAP1</t>
   </si>
   <si>
@@ -253,9 +250,6 @@
   </si>
   <si>
     <t>contains the exclusion criteria to go from D3_SAP1_MS-COHORT to the cohort of women of childbearing age in the DU study</t>
-  </si>
-  <si>
-    <t>07_T3_20_create_selection_criteria_from_SAP1_MS_cohort_to_DU_MS_cohort</t>
   </si>
   <si>
     <t>to be created by R&amp;D</t>
@@ -279,9 +273,6 @@
     <t>contains the exclusion criteria to go from D3_pregnancy to the study population of the pregnant women in the study period, including those with MS</t>
   </si>
   <si>
-    <t>07_T3_40_create_selection_criteria_from_pregnancies</t>
-  </si>
-  <si>
     <t>D3_pregnancy_final D3_DU_MS-COHORT</t>
   </si>
   <si>
@@ -292,9 +283,6 @@
   </si>
   <si>
     <t>counts the pregnancies lost during the selection, per criterion</t>
-  </si>
-  <si>
-    <t>08_T4_50_apply_selection_criteria_to_pregnancies</t>
   </si>
   <si>
     <t>D3_DU_PREGNANCY-COHORT</t>
@@ -328,9 +316,6 @@
   </si>
   <si>
     <t>slug</t>
-  </si>
-  <si>
-    <t>08_T4_30_create_prevalence_MS_in_pregnancy_cohort</t>
   </si>
   <si>
     <r>
@@ -413,10 +398,28 @@
     <t>D5_DU_matching_diagnostic</t>
   </si>
   <si>
-    <t>09_T4_10_match</t>
+    <t>09_T3_10_match</t>
   </si>
   <si>
-    <t>07_T4_30_apply_selection_criteria_to_create_MS-COHORT</t>
+    <t>D3_DU_MS-PREGNANCY-COHORT D3_DU_MS-COHORT</t>
+  </si>
+  <si>
+    <t>07_T2_10_create_MS-COHORT</t>
+  </si>
+  <si>
+    <t>07_T2_20_create_selection_criteria_from_SAP1_MS_cohort_to_DU_MS_cohort</t>
+  </si>
+  <si>
+    <t>07_T3_30_apply_selection_criteria_to_create_MS-COHORT</t>
+  </si>
+  <si>
+    <t>07_T2_40_create_selection_criteria_from_pregnancies</t>
+  </si>
+  <si>
+    <t>07_T3_50_apply_selection_criteria_to_pregnancies</t>
+  </si>
+  <si>
+    <t>08_T3_30_create_prevalence_MS_in_pregnancy_cohort</t>
   </si>
 </sst>
 </file>
@@ -549,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -611,6 +614,10 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -832,10 +839,10 @@
   <dimension ref="A1:AA1025"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A35" sqref="A35"/>
+      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -878,7 +885,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -1375,7 +1382,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="7" t="s">
@@ -1414,7 +1421,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="7" t="s">
@@ -1453,7 +1460,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>51</v>
@@ -1462,7 +1469,7 @@
         <v>52</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="9" t="s">
@@ -1494,7 +1501,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>53</v>
@@ -1503,7 +1510,7 @@
         <v>52</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="9" t="s">
@@ -1535,7 +1542,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>54</v>
@@ -1544,7 +1551,7 @@
         <v>55</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="9" t="s">
@@ -1576,14 +1583,14 @@
         <v>9</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="9" t="s">
@@ -1615,7 +1622,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>57</v>
@@ -1624,7 +1631,7 @@
         <v>58</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="9" t="s">
@@ -1656,14 +1663,14 @@
         <v>9</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="9" t="s">
@@ -1695,7 +1702,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>59</v>
@@ -1704,7 +1711,7 @@
         <v>60</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="9" t="s">
@@ -1736,14 +1743,14 @@
         <v>9</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="9" t="s">
@@ -1775,16 +1782,16 @@
         <v>9</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>61</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="9" t="s">
@@ -1816,16 +1823,16 @@
         <v>9</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>61</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="9" t="s">
@@ -1857,7 +1864,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>62</v>
@@ -1866,7 +1873,7 @@
         <v>63</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="9" t="s">
@@ -1898,16 +1905,16 @@
         <v>9</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>64</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="9" t="s">
@@ -1948,7 +1955,7 @@
         <v>64</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="9" t="s">
@@ -1989,7 +1996,7 @@
         <v>64</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="9" t="s">
@@ -2021,7 +2028,7 @@
         <v>69</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>70</v>
@@ -2030,7 +2037,7 @@
         <v>71</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="9"/>
@@ -2060,7 +2067,7 @@
         <v>69</v>
       </c>
       <c r="B31" s="39" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>70</v>
@@ -2069,7 +2076,7 @@
         <v>71</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="9"/>
@@ -2105,10 +2112,10 @@
         <v>73</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>74</v>
+        <v>124</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -2137,14 +2144,14 @@
       <c r="A33" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="C33" s="27" t="s">
-        <v>77</v>
-      </c>
       <c r="D33" s="28" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="E33" s="29" t="s">
         <v>72</v>
@@ -2153,7 +2160,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="6"/>
       <c r="I33" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -2179,22 +2186,22 @@
         <v>69</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D34" s="28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F34" s="30"/>
       <c r="G34" s="4"/>
       <c r="H34" s="6"/>
       <c r="I34" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -2220,22 +2227,22 @@
         <v>69</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D35" s="28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F35" s="30"/>
       <c r="G35" s="4"/>
       <c r="H35" s="6"/>
       <c r="I35" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -2261,22 +2268,22 @@
         <v>69</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>86</v>
+        <v>127</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="6"/>
       <c r="I36" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -2302,16 +2309,16 @@
         <v>69</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>91</v>
+        <v>128</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -2341,22 +2348,22 @@
         <v>69</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>91</v>
+        <v>128</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="6"/>
       <c r="I38" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -2382,22 +2389,22 @@
         <v>69</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D39" s="32" t="s">
-        <v>91</v>
+        <v>128</v>
       </c>
       <c r="E39" s="33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F39" s="34"/>
       <c r="G39" s="4"/>
       <c r="H39" s="6"/>
       <c r="I39" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -2423,16 +2430,16 @@
         <v>69</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="E40" s="25" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="3" t="s">
@@ -2464,22 +2471,24 @@
         <v>69</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E41" s="25" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
+      <c r="G41" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="H41" s="6"/>
       <c r="I41" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -2505,22 +2514,24 @@
         <v>69</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E42" s="25" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
+      <c r="G42" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="H42" s="6"/>
       <c r="I42" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>

</xml_diff>

<commit_message>
updated intex of codebooks (cleaned SAP1 portion of the program)
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="154">
   <si>
     <t>release</t>
   </si>
@@ -165,13 +165,7 @@
     <t>D5_meaning_occurences</t>
   </si>
   <si>
-    <t>conceptsetdataset 03_T2_20_create_main_components</t>
-  </si>
-  <si>
     <t>D3_main_components D3_study_population_SAP1</t>
-  </si>
-  <si>
-    <t>03_T2_22_create_components_SLE</t>
   </si>
   <si>
     <t>just the dates when persons turn positive for each algorithm if any</t>
@@ -213,9 +207,6 @@
     <t>04_T4_10_create_N_women_and_ranges_MS</t>
   </si>
   <si>
-    <t>05_T5_10_censor_small_count</t>
-  </si>
-  <si>
     <t>Flowchart_exclusion_criteria_masked</t>
   </si>
   <si>
@@ -229,12 +220,6 @@
   </si>
   <si>
     <t>not included yet</t>
-  </si>
-  <si>
-    <t>apply the Cube format to aggregated prevalence of all the MS algorithms in all the study periods and with all the methods</t>
-  </si>
-  <si>
-    <t>06_T3_10_remove_small_counts</t>
   </si>
   <si>
     <t>D3_SAP1_MS-COHORT</t>
@@ -309,28 +294,10 @@
     <t>slug</t>
   </si>
   <si>
-    <r>
-      <t>D3_algorithms_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>MS</t>
-    </r>
-  </si>
-  <si>
     <t>D3_components_MS_SAP1</t>
   </si>
   <si>
     <t>D3_components_multiple_lookback_MS</t>
-  </si>
-  <si>
-    <t>D3_components_MS_SAP1 D3_components_multiple_lookback_MS D3_study_population_SAP1</t>
   </si>
   <si>
     <t>D3_algorithms_multiple_lookback_MS</t>
@@ -373,18 +340,6 @@
   </si>
   <si>
     <t>D5_N_women_and_ranges_MS with masked counts</t>
-  </si>
-  <si>
-    <t>Flowchart_exclusion_criteria D5_meaning_occurences D4_prevalence_aggregated_all_MS D4_prevalence_aggregated_multiple_lookback_MS D5_N_women_and_ranges_MS</t>
-  </si>
-  <si>
-    <t>D4_prevalence_aggregated_MS_selected</t>
-  </si>
-  <si>
-    <t>D4_prevalence_aggregated_all_MS D4_prevalence_aggregated_multiple_lookback_MS</t>
-  </si>
-  <si>
-    <t>D4_prevalence_aggregated_multiple_lookback_MS_selected</t>
   </si>
   <si>
     <t>D5_DU_matching_diagnostic</t>
@@ -464,12 +419,76 @@
   <si>
     <t>D3_DU_selection_criteria_from_pregnancies_to_DU_PREGNANCY-COHORT</t>
   </si>
+  <si>
+    <t>04_T4_30_aggregate_prevalence.R</t>
+  </si>
+  <si>
+    <t>04_T4_20_filter_by_cube_and_calculate_CI.R</t>
+  </si>
+  <si>
+    <t>D5_prevalence_period</t>
+  </si>
+  <si>
+    <t>D5_prevalence_persontime</t>
+  </si>
+  <si>
+    <t>D5_prevalence_average_point</t>
+  </si>
+  <si>
+    <t>D5_prevalence_aggregated_multiple_lookback</t>
+  </si>
+  <si>
+    <t>03_T2_21_create_components_MS</t>
+  </si>
+  <si>
+    <t>03_T2_31_create_algorithms_lookback</t>
+  </si>
+  <si>
+    <t>D3_components_MS_SAP1 D3_components_multiple_lookback_MS</t>
+  </si>
+  <si>
+    <t>D3_algorithms_MS</t>
+  </si>
+  <si>
+    <t>D3_outcomes_cleaned</t>
+  </si>
+  <si>
+    <t>D3_drug_proxies_cleaned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3_study_population_SAP1 D3_outcomes_cleaned D3_drug_proxies_cleaned
+</t>
+  </si>
+  <si>
+    <t>D4_prevalence_period_MS D4_prevalence_persontime_MS D4_prevalence_average_point_MS D4_prevalence_aggregated_multiple_lookback_MS</t>
+  </si>
+  <si>
+    <t>D5_prevalence_period_masked</t>
+  </si>
+  <si>
+    <t>D5_prevalence_persontime_masked</t>
+  </si>
+  <si>
+    <t>D5_prevalence_average_point_masked</t>
+  </si>
+  <si>
+    <t>D5_prevalence_aggregated_multiple_lookback_masked</t>
+  </si>
+  <si>
+    <t>D5_prevalence_aggregated_all</t>
+  </si>
+  <si>
+    <t>D5_prevalence_aggregated_all_masked</t>
+  </si>
+  <si>
+    <t>D5_prevalence_period D5_prevalence_period_masked D5_prevalence_persontime D5_prevalence_persontime_masked D5_prevalence_average_point D5_prevalence_average_point_masked</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -532,8 +551,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -554,20 +580,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF93C47D"/>
-        <bgColor rgb="FF93C47D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB6D7A8"/>
-        <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
     <fill>
@@ -601,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -639,34 +653,41 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -885,21 +906,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA1029"/>
+  <dimension ref="A1:AA1040"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="6.44140625" customWidth="1"/>
-    <col min="2" max="2" width="63.6640625" customWidth="1"/>
-    <col min="3" max="3" width="34.44140625" customWidth="1"/>
-    <col min="4" max="4" width="40.44140625" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="48.77734375" customWidth="1"/>
     <col min="5" max="5" width="46" customWidth="1"/>
     <col min="7" max="7" width="28.33203125" customWidth="1"/>
     <col min="8" max="8" width="18.88671875" customWidth="1"/>
@@ -934,7 +955,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -1231,7 +1252,7 @@
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="36" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="16" t="s">
@@ -1272,7 +1293,7 @@
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="36" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="16"/>
@@ -1308,26 +1329,22 @@
       <c r="AA10" s="4"/>
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>40</v>
+      <c r="A11" s="5"/>
+      <c r="B11" s="23" t="s">
+        <v>62</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>42</v>
+      <c r="D11" s="22" t="s">
+        <v>37</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>43</v>
+      <c r="E11" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="6"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="15"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -1353,14 +1370,16 @@
         <v>9</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
-      <c r="C12" s="14"/>
+      <c r="C12" s="14" t="s">
+        <v>41</v>
+      </c>
       <c r="D12" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
-      <c r="E12" s="19" t="s">
-        <v>46</v>
+      <c r="E12" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="9" t="s">
@@ -1392,18 +1411,18 @@
         <v>9</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="9" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="4"/>
@@ -1430,19 +1449,18 @@
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="40" t="s">
-        <v>97</v>
+      <c r="B14" s="41" t="s">
+        <v>143</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="7" t="s">
-        <v>50</v>
+      <c r="D14" s="22" t="s">
+        <v>45</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="9" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="4"/>
@@ -1470,20 +1488,19 @@
         <v>9</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>98</v>
+        <v>144</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="7" t="s">
-        <v>50</v>
+      <c r="D15" s="22" t="s">
+        <v>45</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="9" t="s">
-        <v>13</v>
+      <c r="G15" s="25" t="s">
+        <v>38</v>
       </c>
-      <c r="H15" s="6"/>
+      <c r="H15" s="15"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -1509,22 +1526,18 @@
         <v>9</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>51</v>
+      <c r="C16" s="14"/>
+      <c r="D16" s="7" t="s">
+        <v>45</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>99</v>
+      <c r="E16" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="6"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="15"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -1546,26 +1559,22 @@
       <c r="AA16" s="4"/>
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>9</v>
+      <c r="A17" s="5"/>
+      <c r="B17" s="23" t="s">
+        <v>64</v>
       </c>
-      <c r="B17" s="25" t="s">
-        <v>100</v>
+      <c r="C17" s="24" t="s">
+        <v>65</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>53</v>
+      <c r="D17" s="22" t="s">
+        <v>45</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>99</v>
+      <c r="E17" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="6"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="15"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -1590,21 +1599,19 @@
       <c r="A18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="25" t="s">
-        <v>101</v>
+      <c r="B18" s="36" t="s">
+        <v>91</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>54</v>
+      <c r="C18" s="14"/>
+      <c r="D18" s="7" t="s">
+        <v>139</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>74</v>
+      <c r="E18" s="19" t="s">
+        <v>48</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="9" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="4"/>
@@ -1632,21 +1639,21 @@
         <v>9</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C19" s="14"/>
-      <c r="D19" s="3" t="s">
-        <v>55</v>
+      <c r="D19" s="22" t="s">
+        <v>139</v>
       </c>
-      <c r="E19" s="20" t="s">
-        <v>74</v>
+      <c r="E19" s="19" t="s">
+        <v>48</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="9" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="H19" s="6"/>
-      <c r="I19" s="3"/>
+      <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
@@ -1655,36 +1662,36 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21"/>
-      <c r="U19" s="21"/>
-      <c r="V19" s="21"/>
-      <c r="W19" s="21"/>
-      <c r="X19" s="21"/>
-      <c r="Y19" s="21"/>
-      <c r="Z19" s="21"/>
-      <c r="AA19" s="21"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>58</v>
+      <c r="D20" s="8" t="s">
+        <v>50</v>
       </c>
-      <c r="E20" s="20" t="s">
-        <v>74</v>
+      <c r="E20" s="14" t="s">
+        <v>141</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="9" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="4"/>
@@ -1707,26 +1714,28 @@
       <c r="Z20" s="4"/>
       <c r="AA20" s="4"/>
     </row>
-    <row r="21" spans="1:27" ht="15.75" customHeight="1">
+    <row r="21" spans="1:27" ht="40.799999999999997" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="37" t="s">
-        <v>104</v>
+      <c r="B21" s="25" t="s">
+        <v>93</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="3" t="s">
-        <v>58</v>
+      <c r="C21" s="14" t="s">
+        <v>51</v>
       </c>
-      <c r="E21" s="20" t="s">
-        <v>74</v>
+      <c r="D21" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>145</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="9" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="H21" s="6"/>
-      <c r="I21" s="3"/>
+      <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
@@ -1735,32 +1744,32 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
-      <c r="Z21" s="21"/>
-      <c r="AA21" s="21"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="9" t="s">
@@ -1791,19 +1800,19 @@
       <c r="A23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="36" t="s">
-        <v>106</v>
+      <c r="B23" s="43" t="s">
+        <v>95</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="3"/>
@@ -1830,17 +1839,17 @@
       <c r="A24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="25" t="s">
-        <v>107</v>
+      <c r="B24" s="43" t="s">
+        <v>96</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>61</v>
+      <c r="D24" s="3" t="s">
+        <v>56</v>
       </c>
-      <c r="E24" s="14" t="s">
-        <v>100</v>
+      <c r="E24" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="9" t="s">
@@ -1871,24 +1880,22 @@
       <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="36" t="s">
-        <v>109</v>
+      <c r="B25" s="43" t="s">
+        <v>97</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>108</v>
+      <c r="C25" s="14"/>
+      <c r="D25" s="3" t="s">
+        <v>56</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>100</v>
+      <c r="E25" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H25" s="6"/>
-      <c r="I25" s="4"/>
+      <c r="I25" s="3"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
@@ -1897,32 +1904,32 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
-      <c r="Z25" s="4"/>
-      <c r="AA25" s="4"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
+      <c r="V25" s="21"/>
+      <c r="W25" s="21"/>
+      <c r="X25" s="21"/>
+      <c r="Y25" s="21"/>
+      <c r="Z25" s="21"/>
+      <c r="AA25" s="21"/>
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1">
       <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="25" t="s">
-        <v>110</v>
+      <c r="B26" s="43" t="s">
+        <v>98</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>63</v>
+      <c r="D26" s="3" t="s">
+        <v>58</v>
       </c>
-      <c r="E26" s="22" t="s">
-        <v>111</v>
+      <c r="E26" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="9" t="s">
@@ -1953,24 +1960,22 @@
       <c r="A27" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="38" t="s">
-        <v>112</v>
+      <c r="B27" s="43" t="s">
+        <v>99</v>
       </c>
-      <c r="C27" s="14" t="s">
-        <v>113</v>
+      <c r="C27" s="14"/>
+      <c r="D27" s="3" t="s">
+        <v>58</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>114</v>
+      <c r="E27" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H27" s="6"/>
-      <c r="I27" s="4"/>
+      <c r="I27" s="3"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
@@ -1979,36 +1984,36 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-      <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
-      <c r="Z27" s="4"/>
-      <c r="AA27" s="4"/>
-    </row>
-    <row r="28" spans="1:27" ht="72">
+      <c r="R27" s="21"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="21"/>
+      <c r="U27" s="21"/>
+      <c r="V27" s="21"/>
+      <c r="W27" s="21"/>
+      <c r="X27" s="21"/>
+      <c r="Y27" s="21"/>
+      <c r="Z27" s="21"/>
+      <c r="AA27" s="21"/>
+    </row>
+    <row r="28" spans="1:27" ht="15.75" customHeight="1">
       <c r="A28" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="23" t="s">
-        <v>65</v>
+      <c r="B28" s="43" t="s">
+        <v>100</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
-      <c r="E28" s="15" t="s">
-        <v>114</v>
+      <c r="E28" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="9" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="4"/>
@@ -2031,25 +2036,25 @@
       <c r="Z28" s="4"/>
       <c r="AA28" s="4"/>
     </row>
-    <row r="29" spans="1:27" ht="72">
+    <row r="29" spans="1:27" ht="15.75" customHeight="1">
       <c r="A29" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="23" t="s">
-        <v>67</v>
+      <c r="B29" s="43" t="s">
+        <v>102</v>
       </c>
-      <c r="C29" s="24" t="s">
-        <v>68</v>
+      <c r="C29" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
-      <c r="E29" s="15" t="s">
-        <v>114</v>
+      <c r="E29" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="4"/>
@@ -2072,26 +2077,28 @@
       <c r="Z29" s="4"/>
       <c r="AA29" s="4"/>
     </row>
-    <row r="30" spans="1:27" ht="57.6">
+    <row r="30" spans="1:27" ht="15.75" customHeight="1">
       <c r="A30" s="5" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
-      <c r="B30" s="39" t="s">
-        <v>115</v>
+      <c r="B30" s="43" t="s">
+        <v>103</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>71</v>
+      <c r="D30" s="8" t="s">
+        <v>61</v>
       </c>
-      <c r="E30" s="14" t="s">
-        <v>116</v>
+      <c r="E30" s="22" t="s">
+        <v>104</v>
       </c>
       <c r="F30" s="4"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="3"/>
+      <c r="G30" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
@@ -2111,26 +2118,24 @@
       <c r="Z30" s="4"/>
       <c r="AA30" s="4"/>
     </row>
-    <row r="31" spans="1:27" ht="57.6">
-      <c r="A31" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" s="39" t="s">
-        <v>117</v>
+    <row r="31" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A31" s="5"/>
+      <c r="B31" s="43" t="s">
+        <v>105</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>71</v>
+      <c r="D31" s="25" t="s">
+        <v>61</v>
       </c>
-      <c r="E31" s="14" t="s">
-        <v>116</v>
+      <c r="E31" s="22" t="s">
+        <v>104</v>
       </c>
       <c r="F31" s="4"/>
-      <c r="G31" s="9"/>
+      <c r="G31" s="25"/>
       <c r="H31" s="15"/>
-      <c r="I31" s="3"/>
+      <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
@@ -2150,26 +2155,22 @@
       <c r="Z31" s="4"/>
       <c r="AA31" s="4"/>
     </row>
-    <row r="32" spans="1:27" ht="43.2">
-      <c r="A32" s="5" t="s">
-        <v>69</v>
+    <row r="32" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A32" s="39"/>
+      <c r="B32" s="43" t="s">
+        <v>135</v>
       </c>
-      <c r="B32" s="25" t="s">
-        <v>72</v>
+      <c r="C32" s="14"/>
+      <c r="D32" s="25" t="s">
+        <v>134</v>
       </c>
-      <c r="C32" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E32" s="24" t="s">
-        <v>74</v>
+      <c r="E32" s="22" t="s">
+        <v>146</v>
       </c>
       <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="3"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
@@ -2189,28 +2190,21 @@
       <c r="Z32" s="4"/>
       <c r="AA32" s="4"/>
     </row>
-    <row r="33" spans="1:27" ht="57.6">
-      <c r="A33" s="5" t="s">
-        <v>69</v>
+    <row r="33" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A33" s="5"/>
+      <c r="B33" s="25" t="s">
+        <v>147</v>
       </c>
-      <c r="B33" s="41" t="s">
-        <v>75</v>
+      <c r="D33" s="25" t="s">
+        <v>134</v>
       </c>
-      <c r="C33" s="42" t="s">
-        <v>76</v>
+      <c r="E33" s="22" t="s">
+        <v>146</v>
       </c>
-      <c r="D33" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="E33" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" s="30"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
@@ -2230,28 +2224,22 @@
       <c r="Z33" s="4"/>
       <c r="AA33" s="4"/>
     </row>
-    <row r="34" spans="1:27" ht="43.2">
-      <c r="A34" s="5" t="s">
-        <v>69</v>
+    <row r="34" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A34" s="5"/>
+      <c r="B34" s="25" t="s">
+        <v>136</v>
       </c>
-      <c r="B34" s="26" t="s">
-        <v>78</v>
+      <c r="C34" s="14"/>
+      <c r="D34" s="25" t="s">
+        <v>134</v>
       </c>
-      <c r="C34" s="27" t="s">
-        <v>79</v>
+      <c r="E34" s="22" t="s">
+        <v>146</v>
       </c>
-      <c r="D34" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="E34" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="F34" s="30"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="F34" s="4"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -2271,28 +2259,21 @@
       <c r="Z34" s="4"/>
       <c r="AA34" s="4"/>
     </row>
-    <row r="35" spans="1:27" ht="28.8">
-      <c r="A35" s="5" t="s">
-        <v>69</v>
+    <row r="35" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A35" s="5"/>
+      <c r="B35" s="25" t="s">
+        <v>148</v>
       </c>
-      <c r="B35" s="28" t="s">
-        <v>80</v>
+      <c r="D35" s="25" t="s">
+        <v>134</v>
       </c>
-      <c r="C35" s="27" t="s">
-        <v>81</v>
+      <c r="E35" s="22" t="s">
+        <v>146</v>
       </c>
-      <c r="D35" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="E35" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="F35" s="30"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="F35" s="4"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
@@ -2312,28 +2293,22 @@
       <c r="Z35" s="4"/>
       <c r="AA35" s="4"/>
     </row>
-    <row r="36" spans="1:27" ht="72">
-      <c r="A36" s="5" t="s">
-        <v>69</v>
+    <row r="36" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A36" s="5"/>
+      <c r="B36" s="25" t="s">
+        <v>137</v>
       </c>
-      <c r="B36" s="25" t="s">
-        <v>143</v>
+      <c r="C36" s="14"/>
+      <c r="D36" s="25" t="s">
+        <v>134</v>
       </c>
-      <c r="C36" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>84</v>
+      <c r="E36" s="22" t="s">
+        <v>146</v>
       </c>
       <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="3" t="s">
-        <v>85</v>
-      </c>
+      <c r="G36" s="25"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
@@ -2353,26 +2328,21 @@
       <c r="Z36" s="4"/>
       <c r="AA36" s="4"/>
     </row>
-    <row r="37" spans="1:27" ht="28.8">
-      <c r="A37" s="5" t="s">
-        <v>69</v>
+    <row r="37" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A37" s="5"/>
+      <c r="B37" s="25" t="s">
+        <v>149</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>142</v>
+      <c r="D37" s="25" t="s">
+        <v>134</v>
       </c>
-      <c r="C37" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>82</v>
+      <c r="E37" s="22" t="s">
+        <v>146</v>
       </c>
       <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="3"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -2392,28 +2362,22 @@
       <c r="Z37" s="4"/>
       <c r="AA37" s="4"/>
     </row>
-    <row r="38" spans="1:27" ht="28.8">
-      <c r="A38" s="5" t="s">
-        <v>69</v>
+    <row r="38" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A38" s="5"/>
+      <c r="B38" s="25" t="s">
+        <v>138</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>137</v>
+      <c r="C38" s="14"/>
+      <c r="D38" s="25" t="s">
+        <v>134</v>
       </c>
-      <c r="C38" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E38" s="25" t="s">
-        <v>82</v>
+      <c r="E38" s="22" t="s">
+        <v>146</v>
       </c>
       <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="3" t="s">
-        <v>85</v>
-      </c>
+      <c r="G38" s="25"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
@@ -2433,28 +2397,21 @@
       <c r="Z38" s="4"/>
       <c r="AA38" s="4"/>
     </row>
-    <row r="39" spans="1:27" ht="43.2">
-      <c r="A39" s="5" t="s">
-        <v>69</v>
+    <row r="39" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A39" s="5"/>
+      <c r="B39" s="25" t="s">
+        <v>150</v>
       </c>
-      <c r="B39" s="32" t="s">
-        <v>141</v>
+      <c r="D39" s="25" t="s">
+        <v>134</v>
       </c>
-      <c r="C39" s="31" t="s">
-        <v>88</v>
+      <c r="E39" s="22" t="s">
+        <v>146</v>
       </c>
-      <c r="D39" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="E39" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="F39" s="34"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="F39" s="4"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
@@ -2474,24 +2431,22 @@
       <c r="Z39" s="4"/>
       <c r="AA39" s="4"/>
     </row>
-    <row r="40" spans="1:27" ht="57.6">
+    <row r="40" spans="1:27" ht="15.75" customHeight="1">
       <c r="A40" s="5"/>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="C40" s="31" t="s">
-        <v>131</v>
+      <c r="E40" s="22" t="s">
+        <v>153</v>
       </c>
-      <c r="D40" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="E40" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="F40" s="34"/>
-      <c r="G40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="25"/>
       <c r="H40" s="15"/>
-      <c r="I40" s="3"/>
+      <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
@@ -2511,24 +2466,22 @@
       <c r="Z40" s="4"/>
       <c r="AA40" s="4"/>
     </row>
-    <row r="41" spans="1:27" ht="86.4">
+    <row r="41" spans="1:27" ht="15.75" customHeight="1">
       <c r="A41" s="5"/>
-      <c r="B41" s="3" t="s">
-        <v>134</v>
+      <c r="B41" s="43" t="s">
+        <v>152</v>
       </c>
-      <c r="C41" s="31" t="s">
-        <v>132</v>
+      <c r="C41" s="14"/>
+      <c r="D41" s="25" t="s">
+        <v>133</v>
       </c>
-      <c r="D41" s="32" t="s">
-        <v>130</v>
+      <c r="E41" s="22" t="s">
+        <v>153</v>
       </c>
-      <c r="E41" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="F41" s="34"/>
-      <c r="G41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="25"/>
       <c r="H41" s="15"/>
-      <c r="I41" s="3"/>
+      <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
@@ -2548,26 +2501,24 @@
       <c r="Z41" s="4"/>
       <c r="AA41" s="4"/>
     </row>
-    <row r="42" spans="1:27" ht="72">
+    <row r="42" spans="1:27" ht="43.2">
       <c r="A42" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E42" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E42" s="25" t="s">
-        <v>128</v>
-      </c>
       <c r="F42" s="4"/>
-      <c r="G42" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="G42" s="4"/>
       <c r="H42" s="6"/>
       <c r="I42" s="3"/>
       <c r="J42" s="4"/>
@@ -2589,22 +2540,28 @@
       <c r="Z42" s="4"/>
       <c r="AA42" s="4"/>
     </row>
-    <row r="43" spans="1:27" ht="14.4">
-      <c r="A43" s="5"/>
-      <c r="B43" s="3" t="s">
-        <v>135</v>
+    <row r="43" spans="1:27" ht="57.6">
+      <c r="A43" s="5" t="s">
+        <v>66</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="3" t="s">
-        <v>129</v>
+      <c r="B43" s="37" t="s">
+        <v>70</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>89</v>
+      <c r="C43" s="38" t="s">
+        <v>71</v>
       </c>
-      <c r="F43" s="4"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="3"/>
+      <c r="D43" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F43" s="30"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
@@ -2624,22 +2581,28 @@
       <c r="Z43" s="4"/>
       <c r="AA43" s="4"/>
     </row>
-    <row r="44" spans="1:27" ht="14.4">
-      <c r="A44" s="5"/>
-      <c r="B44" s="3" t="s">
-        <v>136</v>
+    <row r="44" spans="1:27" ht="43.2">
+      <c r="A44" s="5" t="s">
+        <v>66</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="3" t="s">
-        <v>129</v>
+      <c r="B44" s="26" t="s">
+        <v>73</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>89</v>
+      <c r="C44" s="27" t="s">
+        <v>74</v>
       </c>
-      <c r="F44" s="4"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="3"/>
+      <c r="D44" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E44" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="F44" s="30"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
@@ -2659,29 +2622,27 @@
       <c r="Z44" s="4"/>
       <c r="AA44" s="4"/>
     </row>
-    <row r="45" spans="1:27" ht="86.4">
+    <row r="45" spans="1:27" ht="28.8">
       <c r="A45" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>91</v>
+      <c r="B45" s="28" t="s">
+        <v>75</v>
       </c>
-      <c r="C45" s="15" t="s">
-        <v>92</v>
+      <c r="C45" s="27" t="s">
+        <v>76</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>119</v>
+      <c r="D45" s="28" t="s">
+        <v>112</v>
       </c>
-      <c r="E45" s="25" t="s">
-        <v>120</v>
+      <c r="E45" s="26" t="s">
+        <v>70</v>
       </c>
-      <c r="F45" s="4"/>
-      <c r="G45" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="F45" s="30"/>
+      <c r="G45" s="4"/>
       <c r="H45" s="6"/>
       <c r="I45" s="3" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -2704,27 +2665,25 @@
     </row>
     <row r="46" spans="1:27" ht="72">
       <c r="A46" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>118</v>
+      <c r="B46" s="25" t="s">
+        <v>132</v>
       </c>
-      <c r="C46" s="15" t="s">
-        <v>93</v>
+      <c r="C46" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
-      <c r="E46" s="25" t="s">
-        <v>120</v>
+      <c r="E46" s="20" t="s">
+        <v>79</v>
       </c>
       <c r="F46" s="4"/>
-      <c r="G46" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="G46" s="4"/>
       <c r="H46" s="6"/>
       <c r="I46" s="3" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
@@ -2745,16 +2704,26 @@
       <c r="Z46" s="4"/>
       <c r="AA46" s="4"/>
     </row>
-    <row r="47" spans="1:27" ht="14.4">
-      <c r="A47" s="5"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="6"/>
+    <row r="47" spans="1:27" ht="28.8">
+      <c r="A47" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E47" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
       <c r="H47" s="6"/>
-      <c r="I47" s="4"/>
+      <c r="I47" s="3"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
@@ -2774,16 +2743,28 @@
       <c r="Z47" s="4"/>
       <c r="AA47" s="4"/>
     </row>
-    <row r="48" spans="1:27" ht="14.4">
-      <c r="A48" s="5"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="6"/>
+    <row r="48" spans="1:27" ht="28.8">
+      <c r="A48" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E48" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
       <c r="H48" s="6"/>
-      <c r="I48" s="4"/>
+      <c r="I48" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
@@ -2803,16 +2784,28 @@
       <c r="Z48" s="4"/>
       <c r="AA48" s="4"/>
     </row>
-    <row r="49" spans="1:27" ht="14.4">
-      <c r="A49" s="5"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="4"/>
+    <row r="49" spans="1:27" ht="43.2">
+      <c r="A49" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D49" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="F49" s="34"/>
       <c r="G49" s="4"/>
       <c r="H49" s="6"/>
-      <c r="I49" s="4"/>
+      <c r="I49" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
@@ -2832,16 +2825,26 @@
       <c r="Z49" s="4"/>
       <c r="AA49" s="4"/>
     </row>
-    <row r="50" spans="1:27" ht="14.4">
-      <c r="A50" s="5"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="4"/>
+    <row r="50" spans="1:27" ht="57.6">
+      <c r="A50" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="F50" s="34"/>
       <c r="G50" s="4"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="4"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="3"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
@@ -2861,16 +2864,24 @@
       <c r="Z50" s="4"/>
       <c r="AA50" s="4"/>
     </row>
-    <row r="51" spans="1:27" ht="14.4">
+    <row r="51" spans="1:27" ht="86.4">
       <c r="A51" s="5"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="4"/>
+      <c r="B51" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="D51" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="E51" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="F51" s="34"/>
       <c r="G51" s="4"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="4"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="3"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
@@ -2890,16 +2901,26 @@
       <c r="Z51" s="4"/>
       <c r="AA51" s="4"/>
     </row>
-    <row r="52" spans="1:27" ht="14.4">
-      <c r="A52" s="6"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="6"/>
+    <row r="52" spans="1:27" ht="72">
+      <c r="A52" s="5"/>
+      <c r="B52" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E52" s="25" t="s">
+        <v>117</v>
+      </c>
       <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
+      <c r="G52" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="H52" s="6"/>
-      <c r="I52" s="4"/>
+      <c r="I52" s="3"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
@@ -2920,15 +2941,23 @@
       <c r="AA52" s="4"/>
     </row>
     <row r="53" spans="1:27" ht="14.4">
-      <c r="A53" s="6"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="6"/>
+      <c r="A53" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" s="15"/>
+      <c r="D53" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="4"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="3"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
@@ -2949,15 +2978,21 @@
       <c r="AA53" s="4"/>
     </row>
     <row r="54" spans="1:27" ht="14.4">
-      <c r="A54" s="6"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="6"/>
+      <c r="A54" s="5"/>
+      <c r="B54" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C54" s="15"/>
+      <c r="D54" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="4"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="3"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
@@ -2977,16 +3012,28 @@
       <c r="Z54" s="4"/>
       <c r="AA54" s="4"/>
     </row>
-    <row r="55" spans="1:27" ht="14.4">
-      <c r="A55" s="6"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="6"/>
+    <row r="55" spans="1:27" ht="86.4">
+      <c r="A55" s="5"/>
+      <c r="B55" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E55" s="25" t="s">
+        <v>109</v>
+      </c>
       <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
+      <c r="G55" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="H55" s="6"/>
-      <c r="I55" s="4"/>
+      <c r="I55" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
@@ -3006,16 +3053,30 @@
       <c r="Z55" s="4"/>
       <c r="AA55" s="4"/>
     </row>
-    <row r="56" spans="1:27" ht="14.4">
-      <c r="A56" s="6"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="6"/>
+    <row r="56" spans="1:27" ht="72">
+      <c r="A56" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E56" s="25" t="s">
+        <v>109</v>
+      </c>
       <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
+      <c r="G56" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="H56" s="6"/>
-      <c r="I56" s="4"/>
+      <c r="I56" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
@@ -3036,7 +3097,9 @@
       <c r="AA56" s="4"/>
     </row>
     <row r="57" spans="1:27" ht="14.4">
-      <c r="A57" s="6"/>
+      <c r="A57" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="B57" s="3"/>
       <c r="C57" s="6"/>
       <c r="D57" s="4"/>
@@ -3065,7 +3128,7 @@
       <c r="AA57" s="4"/>
     </row>
     <row r="58" spans="1:27" ht="14.4">
-      <c r="A58" s="6"/>
+      <c r="A58" s="5"/>
       <c r="B58" s="3"/>
       <c r="C58" s="6"/>
       <c r="D58" s="4"/>
@@ -3094,7 +3157,7 @@
       <c r="AA58" s="4"/>
     </row>
     <row r="59" spans="1:27" ht="14.4">
-      <c r="A59" s="6"/>
+      <c r="A59" s="5"/>
       <c r="B59" s="3"/>
       <c r="C59" s="6"/>
       <c r="D59" s="4"/>
@@ -3123,7 +3186,7 @@
       <c r="AA59" s="4"/>
     </row>
     <row r="60" spans="1:27" ht="14.4">
-      <c r="A60" s="6"/>
+      <c r="A60" s="5"/>
       <c r="B60" s="3"/>
       <c r="C60" s="6"/>
       <c r="D60" s="4"/>
@@ -3152,7 +3215,7 @@
       <c r="AA60" s="4"/>
     </row>
     <row r="61" spans="1:27" ht="14.4">
-      <c r="A61" s="6"/>
+      <c r="A61" s="5"/>
       <c r="B61" s="3"/>
       <c r="C61" s="6"/>
       <c r="D61" s="4"/>
@@ -3181,7 +3244,7 @@
       <c r="AA61" s="4"/>
     </row>
     <row r="62" spans="1:27" ht="14.4">
-      <c r="A62" s="6"/>
+      <c r="A62" s="5"/>
       <c r="B62" s="3"/>
       <c r="C62" s="6"/>
       <c r="D62" s="4"/>
@@ -31252,6 +31315,299 @@
       <c r="Z1029" s="4"/>
       <c r="AA1029" s="4"/>
     </row>
+    <row r="1030" spans="1:27" ht="14.4">
+      <c r="A1030" s="6"/>
+      <c r="B1030" s="3"/>
+      <c r="C1030" s="6"/>
+      <c r="D1030" s="4"/>
+      <c r="E1030" s="6"/>
+      <c r="F1030" s="4"/>
+      <c r="G1030" s="4"/>
+      <c r="H1030" s="6"/>
+      <c r="I1030" s="4"/>
+      <c r="J1030" s="4"/>
+      <c r="K1030" s="4"/>
+      <c r="L1030" s="4"/>
+      <c r="M1030" s="4"/>
+      <c r="N1030" s="4"/>
+      <c r="O1030" s="4"/>
+      <c r="P1030" s="4"/>
+      <c r="Q1030" s="4"/>
+      <c r="R1030" s="4"/>
+      <c r="S1030" s="4"/>
+      <c r="T1030" s="4"/>
+      <c r="U1030" s="4"/>
+      <c r="V1030" s="4"/>
+      <c r="W1030" s="4"/>
+      <c r="X1030" s="4"/>
+      <c r="Y1030" s="4"/>
+      <c r="Z1030" s="4"/>
+      <c r="AA1030" s="4"/>
+    </row>
+    <row r="1031" spans="1:27" ht="14.4">
+      <c r="A1031" s="6"/>
+      <c r="B1031" s="3"/>
+      <c r="C1031" s="6"/>
+      <c r="D1031" s="4"/>
+      <c r="E1031" s="6"/>
+      <c r="F1031" s="4"/>
+      <c r="G1031" s="4"/>
+      <c r="H1031" s="6"/>
+      <c r="I1031" s="4"/>
+      <c r="J1031" s="4"/>
+      <c r="K1031" s="4"/>
+      <c r="L1031" s="4"/>
+      <c r="M1031" s="4"/>
+      <c r="N1031" s="4"/>
+      <c r="O1031" s="4"/>
+      <c r="P1031" s="4"/>
+      <c r="Q1031" s="4"/>
+      <c r="R1031" s="4"/>
+      <c r="S1031" s="4"/>
+      <c r="T1031" s="4"/>
+      <c r="U1031" s="4"/>
+      <c r="V1031" s="4"/>
+      <c r="W1031" s="4"/>
+      <c r="X1031" s="4"/>
+      <c r="Y1031" s="4"/>
+      <c r="Z1031" s="4"/>
+      <c r="AA1031" s="4"/>
+    </row>
+    <row r="1032" spans="1:27" ht="14.4">
+      <c r="A1032" s="6"/>
+      <c r="B1032" s="3"/>
+      <c r="C1032" s="6"/>
+      <c r="D1032" s="4"/>
+      <c r="E1032" s="6"/>
+      <c r="F1032" s="4"/>
+      <c r="G1032" s="4"/>
+      <c r="H1032" s="6"/>
+      <c r="I1032" s="4"/>
+      <c r="J1032" s="4"/>
+      <c r="K1032" s="4"/>
+      <c r="L1032" s="4"/>
+      <c r="M1032" s="4"/>
+      <c r="N1032" s="4"/>
+      <c r="O1032" s="4"/>
+      <c r="P1032" s="4"/>
+      <c r="Q1032" s="4"/>
+      <c r="R1032" s="4"/>
+      <c r="S1032" s="4"/>
+      <c r="T1032" s="4"/>
+      <c r="U1032" s="4"/>
+      <c r="V1032" s="4"/>
+      <c r="W1032" s="4"/>
+      <c r="X1032" s="4"/>
+      <c r="Y1032" s="4"/>
+      <c r="Z1032" s="4"/>
+      <c r="AA1032" s="4"/>
+    </row>
+    <row r="1033" spans="1:27" ht="14.4">
+      <c r="A1033" s="6"/>
+      <c r="B1033" s="3"/>
+      <c r="C1033" s="6"/>
+      <c r="D1033" s="4"/>
+      <c r="E1033" s="6"/>
+      <c r="F1033" s="4"/>
+      <c r="G1033" s="4"/>
+      <c r="H1033" s="6"/>
+      <c r="I1033" s="4"/>
+      <c r="J1033" s="4"/>
+      <c r="K1033" s="4"/>
+      <c r="L1033" s="4"/>
+      <c r="M1033" s="4"/>
+      <c r="N1033" s="4"/>
+      <c r="O1033" s="4"/>
+      <c r="P1033" s="4"/>
+      <c r="Q1033" s="4"/>
+      <c r="R1033" s="4"/>
+      <c r="S1033" s="4"/>
+      <c r="T1033" s="4"/>
+      <c r="U1033" s="4"/>
+      <c r="V1033" s="4"/>
+      <c r="W1033" s="4"/>
+      <c r="X1033" s="4"/>
+      <c r="Y1033" s="4"/>
+      <c r="Z1033" s="4"/>
+      <c r="AA1033" s="4"/>
+    </row>
+    <row r="1034" spans="1:27" ht="14.4">
+      <c r="A1034" s="6"/>
+      <c r="B1034" s="3"/>
+      <c r="C1034" s="6"/>
+      <c r="D1034" s="4"/>
+      <c r="E1034" s="6"/>
+      <c r="F1034" s="4"/>
+      <c r="G1034" s="4"/>
+      <c r="H1034" s="6"/>
+      <c r="I1034" s="4"/>
+      <c r="J1034" s="4"/>
+      <c r="K1034" s="4"/>
+      <c r="L1034" s="4"/>
+      <c r="M1034" s="4"/>
+      <c r="N1034" s="4"/>
+      <c r="O1034" s="4"/>
+      <c r="P1034" s="4"/>
+      <c r="Q1034" s="4"/>
+      <c r="R1034" s="4"/>
+      <c r="S1034" s="4"/>
+      <c r="T1034" s="4"/>
+      <c r="U1034" s="4"/>
+      <c r="V1034" s="4"/>
+      <c r="W1034" s="4"/>
+      <c r="X1034" s="4"/>
+      <c r="Y1034" s="4"/>
+      <c r="Z1034" s="4"/>
+      <c r="AA1034" s="4"/>
+    </row>
+    <row r="1035" spans="1:27" ht="14.4">
+      <c r="A1035" s="6"/>
+      <c r="B1035" s="3"/>
+      <c r="C1035" s="6"/>
+      <c r="D1035" s="4"/>
+      <c r="E1035" s="6"/>
+      <c r="F1035" s="4"/>
+      <c r="G1035" s="4"/>
+      <c r="H1035" s="6"/>
+      <c r="I1035" s="4"/>
+      <c r="J1035" s="4"/>
+      <c r="K1035" s="4"/>
+      <c r="L1035" s="4"/>
+      <c r="M1035" s="4"/>
+      <c r="N1035" s="4"/>
+      <c r="O1035" s="4"/>
+      <c r="P1035" s="4"/>
+      <c r="Q1035" s="4"/>
+      <c r="R1035" s="4"/>
+      <c r="S1035" s="4"/>
+      <c r="T1035" s="4"/>
+      <c r="U1035" s="4"/>
+      <c r="V1035" s="4"/>
+      <c r="W1035" s="4"/>
+      <c r="X1035" s="4"/>
+      <c r="Y1035" s="4"/>
+      <c r="Z1035" s="4"/>
+      <c r="AA1035" s="4"/>
+    </row>
+    <row r="1036" spans="1:27" ht="14.4">
+      <c r="A1036" s="6"/>
+      <c r="B1036" s="3"/>
+      <c r="C1036" s="6"/>
+      <c r="D1036" s="4"/>
+      <c r="E1036" s="6"/>
+      <c r="F1036" s="4"/>
+      <c r="G1036" s="4"/>
+      <c r="H1036" s="6"/>
+      <c r="I1036" s="4"/>
+      <c r="J1036" s="4"/>
+      <c r="K1036" s="4"/>
+      <c r="L1036" s="4"/>
+      <c r="M1036" s="4"/>
+      <c r="N1036" s="4"/>
+      <c r="O1036" s="4"/>
+      <c r="P1036" s="4"/>
+      <c r="Q1036" s="4"/>
+      <c r="R1036" s="4"/>
+      <c r="S1036" s="4"/>
+      <c r="T1036" s="4"/>
+      <c r="U1036" s="4"/>
+      <c r="V1036" s="4"/>
+      <c r="W1036" s="4"/>
+      <c r="X1036" s="4"/>
+      <c r="Y1036" s="4"/>
+      <c r="Z1036" s="4"/>
+      <c r="AA1036" s="4"/>
+    </row>
+    <row r="1037" spans="1:27" ht="14.4">
+      <c r="A1037" s="6"/>
+      <c r="B1037" s="3"/>
+      <c r="C1037" s="6"/>
+      <c r="D1037" s="4"/>
+      <c r="E1037" s="6"/>
+      <c r="F1037" s="4"/>
+      <c r="G1037" s="4"/>
+      <c r="H1037" s="6"/>
+      <c r="I1037" s="4"/>
+      <c r="J1037" s="4"/>
+      <c r="K1037" s="4"/>
+      <c r="L1037" s="4"/>
+      <c r="M1037" s="4"/>
+      <c r="N1037" s="4"/>
+      <c r="O1037" s="4"/>
+      <c r="P1037" s="4"/>
+      <c r="Q1037" s="4"/>
+      <c r="R1037" s="4"/>
+      <c r="S1037" s="4"/>
+      <c r="T1037" s="4"/>
+      <c r="U1037" s="4"/>
+      <c r="V1037" s="4"/>
+      <c r="W1037" s="4"/>
+      <c r="X1037" s="4"/>
+      <c r="Y1037" s="4"/>
+      <c r="Z1037" s="4"/>
+      <c r="AA1037" s="4"/>
+    </row>
+    <row r="1038" spans="1:27" ht="14.4">
+      <c r="A1038" s="6"/>
+      <c r="B1038" s="3"/>
+      <c r="C1038" s="6"/>
+      <c r="D1038" s="4"/>
+      <c r="E1038" s="6"/>
+      <c r="F1038" s="4"/>
+      <c r="G1038" s="4"/>
+      <c r="H1038" s="6"/>
+      <c r="I1038" s="4"/>
+      <c r="J1038" s="4"/>
+      <c r="K1038" s="4"/>
+      <c r="L1038" s="4"/>
+      <c r="M1038" s="4"/>
+      <c r="N1038" s="4"/>
+      <c r="O1038" s="4"/>
+      <c r="P1038" s="4"/>
+      <c r="Q1038" s="4"/>
+      <c r="R1038" s="4"/>
+      <c r="S1038" s="4"/>
+      <c r="T1038" s="4"/>
+      <c r="U1038" s="4"/>
+      <c r="V1038" s="4"/>
+      <c r="W1038" s="4"/>
+      <c r="X1038" s="4"/>
+      <c r="Y1038" s="4"/>
+      <c r="Z1038" s="4"/>
+      <c r="AA1038" s="4"/>
+    </row>
+    <row r="1039" spans="1:27" ht="14.4">
+      <c r="A1039" s="6"/>
+      <c r="B1039" s="3"/>
+      <c r="C1039" s="6"/>
+      <c r="D1039" s="4"/>
+      <c r="E1039" s="6"/>
+      <c r="F1039" s="4"/>
+      <c r="G1039" s="4"/>
+      <c r="H1039" s="6"/>
+      <c r="I1039" s="4"/>
+      <c r="J1039" s="4"/>
+      <c r="K1039" s="4"/>
+      <c r="L1039" s="4"/>
+      <c r="M1039" s="4"/>
+      <c r="N1039" s="4"/>
+      <c r="O1039" s="4"/>
+      <c r="P1039" s="4"/>
+      <c r="Q1039" s="4"/>
+      <c r="R1039" s="4"/>
+      <c r="S1039" s="4"/>
+      <c r="T1039" s="4"/>
+      <c r="U1039" s="4"/>
+      <c r="V1039" s="4"/>
+      <c r="W1039" s="4"/>
+      <c r="X1039" s="4"/>
+      <c r="Y1039" s="4"/>
+      <c r="Z1039" s="4"/>
+      <c r="AA1039" s="4"/>
+    </row>
+    <row r="1040" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A1040" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
codebooks for DU cohorts and for DU template 1 and 2
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="152">
   <si>
     <t>release</t>
   </si>
@@ -240,9 +240,6 @@
     <t>to be created by R&amp;D</t>
   </si>
   <si>
-    <t>D3_DU_MS-COHORT</t>
-  </si>
-  <si>
     <t>contains the cohort of women of childbearing age included in the DU study</t>
   </si>
   <si>
@@ -258,19 +255,10 @@
     <t>contains the exclusion criteria to go from D3_pregnancy to the study population of the pregnant women in the study period, including those with MS</t>
   </si>
   <si>
-    <t>D3_pregnancy_final D3_DU_MS-COHORT</t>
-  </si>
-  <si>
     <t>created by R&amp;D</t>
   </si>
   <si>
     <t>counts the pregnancies lost during the selection, per criterion</t>
-  </si>
-  <si>
-    <t>contains the cohort of pregnancies included in the study</t>
-  </si>
-  <si>
-    <t>contains the cohort of pregnancies included in the study that have MS during the pregnancy study period</t>
   </si>
   <si>
     <t>D4_DU_prevalence_MS_in_pregnancy_cohort</t>
@@ -351,21 +339,6 @@
     <t>D3_DU_MS-PREGNANCY-COHORT D3_DU_MS-COHORT</t>
   </si>
   <si>
-    <t>07_T2_10_create_MS-COHORT</t>
-  </si>
-  <si>
-    <t>07_T2_20_create_selection_criteria_from_SAP1_MS_cohort_to_DU_MS_cohort</t>
-  </si>
-  <si>
-    <t>07_T3_30_apply_selection_criteria_to_create_MS-COHORT</t>
-  </si>
-  <si>
-    <t>07_T2_40_create_selection_criteria_from_pregnancies</t>
-  </si>
-  <si>
-    <t>07_T3_50_apply_selection_criteria_to_pregnancies</t>
-  </si>
-  <si>
     <t>08_T3_30_create_prevalence_MS_in_pregnancy_cohort</t>
   </si>
   <si>
@@ -376,9 +349,6 @@
   </si>
   <si>
     <t>08_T4_40_create_templates_on_prevalence_MS_in_pregnancy_cohort</t>
-  </si>
-  <si>
-    <t>08_T4_20_create_descriptives_pregnancies_M</t>
   </si>
   <si>
     <t>numbers to be included in Template 1:  Description of the time period between 2 pregnancies in the pregnancy cohort and in the MS-pregnancy cohort</t>
@@ -400,12 +370,6 @@
   </si>
   <si>
     <t>D4_DU_PREGNANCY-COHORT</t>
-  </si>
-  <si>
-    <t>D3_DU_PREGNANCY-COHORT_all</t>
-  </si>
-  <si>
-    <t>07_T2_60_collect_variables_for_pregnancies</t>
   </si>
   <si>
     <t>D4_DU_PREGNANCY-COHORT D3_DU_MS-COHORT D3_study_population_SAP1</t>
@@ -483,6 +447,36 @@
   <si>
     <t>D5_prevalence_period D5_prevalence_period_masked D5_prevalence_persontime D5_prevalence_persontime_masked D5_prevalence_average_point D5_prevalence_average_point_masked</t>
   </si>
+  <si>
+    <t>05_T2_10_create_MS-COHORT</t>
+  </si>
+  <si>
+    <t>05_T2_20_create_selection_criteria_from_SAP1_MS_cohort_to_DU_MS_cohort</t>
+  </si>
+  <si>
+    <t>contains the cohort of pregnancies included in the study, with variables</t>
+  </si>
+  <si>
+    <t>D3_pregnancy_final D3_study_population_SAP1</t>
+  </si>
+  <si>
+    <t>05_T2_30_create_selection_criteria_from_pregnancies</t>
+  </si>
+  <si>
+    <t>06_T3_10_apply_selection_criteria_to_create_MS-COHORT</t>
+  </si>
+  <si>
+    <t>06_T3_20_apply_selection_criteria_to_pregnancies</t>
+  </si>
+  <si>
+    <t>D4_DU_MS-COHORT</t>
+  </si>
+  <si>
+    <t>07_T2_10_collect_variables_for_pregnancies</t>
+  </si>
+  <si>
+    <t>08_T4_20_create_descriptives_pregnancies</t>
+  </si>
 </sst>
 </file>
 
@@ -559,7 +553,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -590,18 +584,6 @@
         <bgColor rgb="FF6AA84F"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF9CB9C"/>
-        <bgColor rgb="FFF9CB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFCE5CD"/>
-        <bgColor rgb="FFFCE5CD"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -615,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -658,25 +640,8 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -688,6 +653,21 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -909,10 +889,10 @@
   <dimension ref="A1:AA1040"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
+      <selection pane="bottomRight" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -954,8 +934,8 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="35" t="s">
-        <v>90</v>
+      <c r="J1" s="26" t="s">
+        <v>86</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -1252,7 +1232,7 @@
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="27" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="16" t="s">
@@ -1293,7 +1273,7 @@
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="27" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="16"/>
@@ -1449,8 +1429,8 @@
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="41" t="s">
-        <v>143</v>
+      <c r="B14" s="30" t="s">
+        <v>131</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>45</v>
@@ -1487,8 +1467,8 @@
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="40" t="s">
-        <v>144</v>
+      <c r="B15" s="29" t="s">
+        <v>132</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>45</v>
@@ -1599,12 +1579,12 @@
       <c r="A18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="36" t="s">
-        <v>91</v>
+      <c r="B18" s="27" t="s">
+        <v>87</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="7" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>48</v>
@@ -1638,12 +1618,12 @@
       <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="36" t="s">
-        <v>92</v>
+      <c r="B19" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="22" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>48</v>
@@ -1678,7 +1658,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>49</v>
@@ -1687,7 +1667,7 @@
         <v>50</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="9" t="s">
@@ -1719,16 +1699,16 @@
         <v>9</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
-      <c r="E21" s="42" t="s">
-        <v>145</v>
+      <c r="E21" s="31" t="s">
+        <v>133</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="9" t="s">
@@ -1760,7 +1740,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>52</v>
@@ -1800,8 +1780,8 @@
       <c r="A23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="43" t="s">
-        <v>95</v>
+      <c r="B23" s="32" t="s">
+        <v>91</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="3" t="s">
@@ -1839,8 +1819,8 @@
       <c r="A24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="43" t="s">
-        <v>96</v>
+      <c r="B24" s="32" t="s">
+        <v>92</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>55</v>
@@ -1880,8 +1860,8 @@
       <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="43" t="s">
-        <v>97</v>
+      <c r="B25" s="32" t="s">
+        <v>93</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="3" t="s">
@@ -1919,8 +1899,8 @@
       <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="43" t="s">
-        <v>98</v>
+      <c r="B26" s="32" t="s">
+        <v>94</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>57</v>
@@ -1960,8 +1940,8 @@
       <c r="A27" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="43" t="s">
-        <v>99</v>
+      <c r="B27" s="32" t="s">
+        <v>95</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="3" t="s">
@@ -1999,17 +1979,17 @@
       <c r="A28" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="43" t="s">
-        <v>100</v>
+      <c r="B28" s="32" t="s">
+        <v>96</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>59</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="9" t="s">
@@ -2040,17 +2020,17 @@
       <c r="A29" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="43" t="s">
-        <v>102</v>
+      <c r="B29" s="32" t="s">
+        <v>98</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>59</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="9" t="s">
@@ -2081,8 +2061,8 @@
       <c r="A30" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="43" t="s">
-        <v>103</v>
+      <c r="B30" s="32" t="s">
+        <v>99</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>60</v>
@@ -2091,7 +2071,7 @@
         <v>61</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="9" t="s">
@@ -2120,17 +2100,17 @@
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
       <c r="A31" s="5"/>
-      <c r="B31" s="43" t="s">
-        <v>105</v>
+      <c r="B31" s="32" t="s">
+        <v>101</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D31" s="25" t="s">
         <v>61</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="25"/>
@@ -2156,16 +2136,16 @@
       <c r="AA31" s="4"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A32" s="39"/>
-      <c r="B32" s="43" t="s">
-        <v>135</v>
+      <c r="A32" s="28"/>
+      <c r="B32" s="32" t="s">
+        <v>123</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="25" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="25"/>
@@ -2193,13 +2173,13 @@
     <row r="33" spans="1:27" ht="15.75" customHeight="1">
       <c r="A33" s="5"/>
       <c r="B33" s="25" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="25"/>
@@ -2227,14 +2207,14 @@
     <row r="34" spans="1:27" ht="15.75" customHeight="1">
       <c r="A34" s="5"/>
       <c r="B34" s="25" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C34" s="14"/>
       <c r="D34" s="25" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="25"/>
@@ -2262,13 +2242,13 @@
     <row r="35" spans="1:27" ht="15.75" customHeight="1">
       <c r="A35" s="5"/>
       <c r="B35" s="25" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="25"/>
@@ -2296,14 +2276,14 @@
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
       <c r="A36" s="5"/>
       <c r="B36" s="25" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="25" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="25"/>
@@ -2331,13 +2311,13 @@
     <row r="37" spans="1:27" ht="15.75" customHeight="1">
       <c r="A37" s="5"/>
       <c r="B37" s="25" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="25"/>
@@ -2365,14 +2345,14 @@
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
       <c r="A38" s="5"/>
       <c r="B38" s="25" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C38" s="14"/>
       <c r="D38" s="25" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="25"/>
@@ -2400,13 +2380,13 @@
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
       <c r="A39" s="5"/>
       <c r="B39" s="25" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="25"/>
@@ -2433,15 +2413,15 @@
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
       <c r="A40" s="5"/>
-      <c r="B40" s="43" t="s">
-        <v>151</v>
+      <c r="B40" s="32" t="s">
+        <v>139</v>
       </c>
       <c r="C40" s="14"/>
       <c r="D40" s="25" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="25"/>
@@ -2468,15 +2448,15 @@
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
       <c r="A41" s="5"/>
-      <c r="B41" s="43" t="s">
-        <v>152</v>
+      <c r="B41" s="32" t="s">
+        <v>140</v>
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="25" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="25"/>
@@ -2501,7 +2481,7 @@
       <c r="Z41" s="4"/>
       <c r="AA41" s="4"/>
     </row>
-    <row r="42" spans="1:27" ht="43.2">
+    <row r="42" spans="1:27" ht="72">
       <c r="A42" s="5" t="s">
         <v>66</v>
       </c>
@@ -2512,7 +2492,7 @@
         <v>68</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="E42" s="24" t="s">
         <v>69</v>
@@ -2540,7 +2520,7 @@
       <c r="Z42" s="4"/>
       <c r="AA42" s="4"/>
     </row>
-    <row r="43" spans="1:27" ht="57.6">
+    <row r="43" spans="1:27" ht="86.4">
       <c r="A43" s="5" t="s">
         <v>66</v>
       </c>
@@ -2550,13 +2530,13 @@
       <c r="C43" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D43" s="28" t="s">
-        <v>111</v>
+      <c r="D43" s="33" t="s">
+        <v>143</v>
       </c>
-      <c r="E43" s="29" t="s">
+      <c r="E43" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="F43" s="30"/>
+      <c r="F43" s="35"/>
       <c r="G43" s="4"/>
       <c r="H43" s="6"/>
       <c r="I43" s="3" t="s">
@@ -2581,27 +2561,27 @@
       <c r="Z43" s="4"/>
       <c r="AA43" s="4"/>
     </row>
-    <row r="44" spans="1:27" ht="43.2">
+    <row r="44" spans="1:27" ht="100.8">
       <c r="A44" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B44" s="26" t="s">
-        <v>73</v>
+      <c r="B44" s="32" t="s">
+        <v>120</v>
       </c>
-      <c r="C44" s="27" t="s">
-        <v>74</v>
+      <c r="C44" s="40" t="s">
+        <v>77</v>
       </c>
-      <c r="D44" s="28" t="s">
-        <v>112</v>
+      <c r="D44" s="33" t="s">
+        <v>146</v>
       </c>
-      <c r="E44" s="26" t="s">
-        <v>116</v>
+      <c r="E44" s="41" t="s">
+        <v>145</v>
       </c>
-      <c r="F44" s="30"/>
+      <c r="F44" s="35"/>
       <c r="G44" s="4"/>
       <c r="H44" s="6"/>
       <c r="I44" s="3" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -2622,23 +2602,23 @@
       <c r="Z44" s="4"/>
       <c r="AA44" s="4"/>
     </row>
-    <row r="45" spans="1:27" ht="28.8">
+    <row r="45" spans="1:27" ht="57.6">
       <c r="A45" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="28" t="s">
-        <v>75</v>
+      <c r="B45" s="32" t="s">
+        <v>149</v>
       </c>
-      <c r="C45" s="27" t="s">
-        <v>76</v>
+      <c r="C45" s="40" t="s">
+        <v>73</v>
       </c>
-      <c r="D45" s="28" t="s">
-        <v>112</v>
+      <c r="D45" s="33" t="s">
+        <v>147</v>
       </c>
-      <c r="E45" s="26" t="s">
-        <v>70</v>
+      <c r="E45" s="32" t="s">
+        <v>107</v>
       </c>
-      <c r="F45" s="30"/>
+      <c r="F45" s="35"/>
       <c r="G45" s="4"/>
       <c r="H45" s="6"/>
       <c r="I45" s="3" t="s">
@@ -2663,27 +2643,27 @@
       <c r="Z45" s="4"/>
       <c r="AA45" s="4"/>
     </row>
-    <row r="46" spans="1:27" ht="72">
+    <row r="46" spans="1:27" ht="43.2">
       <c r="A46" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B46" s="25" t="s">
-        <v>132</v>
+      <c r="B46" s="33" t="s">
+        <v>74</v>
       </c>
-      <c r="C46" s="14" t="s">
-        <v>78</v>
+      <c r="C46" s="40" t="s">
+        <v>75</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>113</v>
+      <c r="D46" s="33" t="s">
+        <v>147</v>
       </c>
-      <c r="E46" s="20" t="s">
-        <v>79</v>
+      <c r="E46" s="32" t="s">
+        <v>70</v>
       </c>
-      <c r="F46" s="4"/>
+      <c r="F46" s="35"/>
       <c r="G46" s="4"/>
       <c r="H46" s="6"/>
       <c r="I46" s="3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
@@ -2704,67 +2684,37 @@
       <c r="Z46" s="4"/>
       <c r="AA46" s="4"/>
     </row>
-    <row r="47" spans="1:27" ht="28.8">
-      <c r="A47" s="5" t="s">
-        <v>66</v>
-      </c>
+    <row r="47" spans="1:27" ht="15.75" customHeight="1">
       <c r="B47" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
-      <c r="S47" s="4"/>
-      <c r="T47" s="4"/>
-      <c r="U47" s="4"/>
-      <c r="V47" s="4"/>
-      <c r="W47" s="4"/>
-      <c r="X47" s="4"/>
-      <c r="Y47" s="4"/>
-      <c r="Z47" s="4"/>
-      <c r="AA47" s="4"/>
-    </row>
-    <row r="48" spans="1:27" ht="28.8">
+    </row>
+    <row r="48" spans="1:27" ht="43.2">
       <c r="A48" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
       <c r="H48" s="6"/>
-      <c r="I48" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="I48" s="3"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
@@ -2784,23 +2734,23 @@
       <c r="Z48" s="4"/>
       <c r="AA48" s="4"/>
     </row>
-    <row r="49" spans="1:27" ht="43.2">
+    <row r="49" spans="1:27" ht="14.4">
       <c r="A49" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B49" s="32" t="s">
-        <v>130</v>
+      <c r="B49" s="33" t="s">
+        <v>118</v>
       </c>
-      <c r="C49" s="31" t="s">
-        <v>83</v>
+      <c r="C49" s="34" t="s">
+        <v>144</v>
       </c>
-      <c r="D49" s="32" t="s">
-        <v>128</v>
+      <c r="D49" s="33" t="s">
+        <v>150</v>
       </c>
-      <c r="E49" s="33" t="s">
-        <v>129</v>
+      <c r="E49" s="32" t="s">
+        <v>117</v>
       </c>
-      <c r="F49" s="34"/>
+      <c r="F49" s="35"/>
       <c r="G49" s="4"/>
       <c r="H49" s="6"/>
       <c r="I49" s="3" t="s">
@@ -2825,23 +2775,23 @@
       <c r="Z49" s="4"/>
       <c r="AA49" s="4"/>
     </row>
-    <row r="50" spans="1:27" ht="57.6">
+    <row r="50" spans="1:27" ht="115.2">
       <c r="A50" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>122</v>
+      <c r="B50" s="33" t="s">
+        <v>112</v>
       </c>
-      <c r="C50" s="31" t="s">
-        <v>120</v>
+      <c r="C50" s="36" t="s">
+        <v>110</v>
       </c>
-      <c r="D50" s="32" t="s">
-        <v>119</v>
+      <c r="D50" s="33" t="s">
+        <v>151</v>
       </c>
       <c r="E50" s="33" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
-      <c r="F50" s="34"/>
+      <c r="F50" s="35"/>
       <c r="G50" s="4"/>
       <c r="H50" s="15"/>
       <c r="I50" s="3"/>
@@ -2864,21 +2814,21 @@
       <c r="Z50" s="4"/>
       <c r="AA50" s="4"/>
     </row>
-    <row r="51" spans="1:27" ht="86.4">
+    <row r="51" spans="1:27" ht="144">
       <c r="A51" s="5"/>
-      <c r="B51" s="3" t="s">
-        <v>123</v>
+      <c r="B51" s="33" t="s">
+        <v>113</v>
       </c>
-      <c r="C51" s="31" t="s">
-        <v>121</v>
+      <c r="C51" s="36" t="s">
+        <v>111</v>
       </c>
-      <c r="D51" s="32" t="s">
-        <v>119</v>
+      <c r="D51" s="33" t="s">
+        <v>151</v>
       </c>
       <c r="E51" s="33" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
-      <c r="F51" s="34"/>
+      <c r="F51" s="35"/>
       <c r="G51" s="4"/>
       <c r="H51" s="15"/>
       <c r="I51" s="3"/>
@@ -2901,19 +2851,19 @@
       <c r="Z51" s="4"/>
       <c r="AA51" s="4"/>
     </row>
-    <row r="52" spans="1:27" ht="72">
+    <row r="52" spans="1:27" ht="144">
       <c r="A52" s="5"/>
       <c r="B52" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E52" s="25" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="3" t="s">
@@ -2945,14 +2895,14 @@
         <v>66</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C53" s="15"/>
       <c r="D53" s="3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="3"/>
@@ -2980,14 +2930,14 @@
     <row r="54" spans="1:27" ht="14.4">
       <c r="A54" s="5"/>
       <c r="B54" s="3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C54" s="15"/>
       <c r="D54" s="3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="3"/>
@@ -3012,19 +2962,19 @@
       <c r="Z54" s="4"/>
       <c r="AA54" s="4"/>
     </row>
-    <row r="55" spans="1:27" ht="86.4">
+    <row r="55" spans="1:27" ht="158.4">
       <c r="A55" s="5"/>
       <c r="B55" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E55" s="25" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="3" t="s">
@@ -3032,7 +2982,7 @@
       </c>
       <c r="H55" s="6"/>
       <c r="I55" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
@@ -3053,21 +3003,21 @@
       <c r="Z55" s="4"/>
       <c r="AA55" s="4"/>
     </row>
-    <row r="56" spans="1:27" ht="72">
+    <row r="56" spans="1:27" ht="100.8">
       <c r="A56" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E56" s="25" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="3" t="s">
@@ -3075,7 +3025,7 @@
       </c>
       <c r="H56" s="6"/>
       <c r="I56" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>

</xml_diff>

<commit_message>
codebooks for Template 4 and 5
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="155">
   <si>
     <t>release</t>
   </si>
@@ -264,9 +264,6 @@
     <t>D4_DU_prevalence_MS_in_pregnancy_cohort</t>
   </si>
   <si>
-    <t>contains the aggregated prevalence (numerators and denominators) needed to compute prevalence of MS in the pregnancy cohort, to feed Template 4 and 5this is to feed Template 4 and 5</t>
-  </si>
-  <si>
     <t>D4_DU_matched_MS-PREGNANCY-COHORT_to_MS-COHORT</t>
   </si>
   <si>
@@ -343,9 +340,6 @@
   </si>
   <si>
     <t>D3_DU_selection_criteria_from_SAP1_MS_cohort_to_DU_MS_cohort D3_SAP1_MS-COHORT</t>
-  </si>
-  <si>
-    <t>D3_DU_MS-PREGNANCY-COHORT D3_DU_PREGNANCY-COHORT</t>
   </si>
   <si>
     <t>08_T4_40_create_templates_on_prevalence_MS_in_pregnancy_cohort</t>
@@ -476,6 +470,21 @@
   </si>
   <si>
     <t>08_T4_20_create_descriptives_pregnancies</t>
+  </si>
+  <si>
+    <t>D3_candidate_matches_MS_non_pregnant</t>
+  </si>
+  <si>
+    <t>09_create_candidate_matches_MS_non_pregnant</t>
+  </si>
+  <si>
+    <t>contains the aggregated prevalence (numerators and denominators) needed to compute prevalence of MS in the pregnancy cohort, to feed Template 4 and 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This applies some of the steps in the appendix: all the </t>
+  </si>
+  <si>
+    <t>Prevalence of MS over time per 1,000 pregnancies from women aged 15-49 years old</t>
   </si>
 </sst>
 </file>
@@ -889,10 +898,10 @@
   <dimension ref="A1:AA1040"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E48" sqref="E48"/>
+      <selection pane="bottomRight" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -935,7 +944,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -1430,7 +1439,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>45</v>
@@ -1468,7 +1477,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>45</v>
@@ -1580,11 +1589,11 @@
         <v>9</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>48</v>
@@ -1619,11 +1628,11 @@
         <v>9</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>48</v>
@@ -1658,7 +1667,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>49</v>
@@ -1667,7 +1676,7 @@
         <v>50</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="9" t="s">
@@ -1699,16 +1708,16 @@
         <v>9</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="9" t="s">
@@ -1740,7 +1749,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>52</v>
@@ -1781,7 +1790,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="3" t="s">
@@ -1820,7 +1829,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>55</v>
@@ -1861,7 +1870,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="3" t="s">
@@ -1900,7 +1909,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>57</v>
@@ -1941,7 +1950,7 @@
         <v>9</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="3" t="s">
@@ -1980,16 +1989,16 @@
         <v>9</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>59</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="9" t="s">
@@ -2021,16 +2030,16 @@
         <v>9</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>59</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="9" t="s">
@@ -2062,7 +2071,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>60</v>
@@ -2071,7 +2080,7 @@
         <v>61</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="9" t="s">
@@ -2101,16 +2110,16 @@
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
       <c r="A31" s="5"/>
       <c r="B31" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D31" s="25" t="s">
         <v>61</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="25"/>
@@ -2138,14 +2147,14 @@
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
       <c r="A32" s="28"/>
       <c r="B32" s="32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="25"/>
@@ -2173,13 +2182,13 @@
     <row r="33" spans="1:27" ht="15.75" customHeight="1">
       <c r="A33" s="5"/>
       <c r="B33" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="25"/>
@@ -2207,14 +2216,14 @@
     <row r="34" spans="1:27" ht="15.75" customHeight="1">
       <c r="A34" s="5"/>
       <c r="B34" s="25" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C34" s="14"/>
       <c r="D34" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="25"/>
@@ -2242,13 +2251,13 @@
     <row r="35" spans="1:27" ht="15.75" customHeight="1">
       <c r="A35" s="5"/>
       <c r="B35" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="25"/>
@@ -2276,14 +2285,14 @@
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
       <c r="A36" s="5"/>
       <c r="B36" s="25" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="25"/>
@@ -2311,13 +2320,13 @@
     <row r="37" spans="1:27" ht="15.75" customHeight="1">
       <c r="A37" s="5"/>
       <c r="B37" s="25" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="25"/>
@@ -2345,14 +2354,14 @@
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
       <c r="A38" s="5"/>
       <c r="B38" s="25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C38" s="14"/>
       <c r="D38" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="25"/>
@@ -2380,13 +2389,13 @@
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
       <c r="A39" s="5"/>
       <c r="B39" s="25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="25"/>
@@ -2414,14 +2423,14 @@
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="32" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C40" s="14"/>
       <c r="D40" s="25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="25"/>
@@ -2449,14 +2458,14 @@
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
       <c r="A41" s="5"/>
       <c r="B41" s="32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="25"/>
@@ -2492,7 +2501,7 @@
         <v>68</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E42" s="24" t="s">
         <v>69</v>
@@ -2531,7 +2540,7 @@
         <v>71</v>
       </c>
       <c r="D43" s="33" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E43" s="39" t="s">
         <v>67</v>
@@ -2566,16 +2575,16 @@
         <v>66</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C44" s="40" t="s">
         <v>77</v>
       </c>
       <c r="D44" s="33" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E44" s="41" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F44" s="35"/>
       <c r="G44" s="4"/>
@@ -2607,16 +2616,16 @@
         <v>66</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C45" s="40" t="s">
         <v>73</v>
       </c>
       <c r="D45" s="33" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F45" s="35"/>
       <c r="G45" s="4"/>
@@ -2654,7 +2663,7 @@
         <v>75</v>
       </c>
       <c r="D46" s="33" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E46" s="32" t="s">
         <v>70</v>
@@ -2686,10 +2695,10 @@
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
       <c r="B47" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E47" s="25" t="s">
         <v>76</v>
@@ -2700,13 +2709,13 @@
         <v>66</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>79</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E48" s="25" t="s">
         <v>76</v>
@@ -2739,16 +2748,16 @@
         <v>66</v>
       </c>
       <c r="B49" s="33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C49" s="34" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D49" s="33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E49" s="32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F49" s="35"/>
       <c r="G49" s="4"/>
@@ -2780,16 +2789,16 @@
         <v>66</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C50" s="36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D50" s="33" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E50" s="33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F50" s="35"/>
       <c r="G50" s="4"/>
@@ -2817,16 +2826,16 @@
     <row r="51" spans="1:27" ht="144">
       <c r="A51" s="5"/>
       <c r="B51" s="33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C51" s="36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D51" s="33" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E51" s="33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F51" s="35"/>
       <c r="G51" s="4"/>
@@ -2851,19 +2860,19 @@
       <c r="Z51" s="4"/>
       <c r="AA51" s="4"/>
     </row>
-    <row r="52" spans="1:27" ht="144">
+    <row r="52" spans="1:27" ht="115.2">
       <c r="A52" s="5"/>
       <c r="B52" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>81</v>
+        <v>152</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
-      <c r="E52" s="25" t="s">
-        <v>108</v>
+      <c r="E52" s="33" t="s">
+        <v>116</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="3" t="s">
@@ -2895,11 +2904,13 @@
         <v>66</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
-      <c r="C53" s="15"/>
+      <c r="C53" s="25" t="s">
+        <v>154</v>
+      </c>
       <c r="D53" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>80</v>
@@ -2930,11 +2941,11 @@
     <row r="54" spans="1:27" ht="14.4">
       <c r="A54" s="5"/>
       <c r="B54" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C54" s="15"/>
       <c r="D54" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>80</v>
@@ -2962,120 +2973,16 @@
       <c r="Z54" s="4"/>
       <c r="AA54" s="4"/>
     </row>
-    <row r="55" spans="1:27" ht="158.4">
-      <c r="A55" s="5"/>
+    <row r="55" spans="1:27" ht="15.75" customHeight="1">
       <c r="B55" s="3" t="s">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>83</v>
+        <v>153</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>104</v>
+        <v>151</v>
       </c>
-      <c r="E55" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="F55" s="4"/>
-      <c r="G55" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H55" s="6"/>
-      <c r="I55" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
-      <c r="P55" s="4"/>
-      <c r="Q55" s="4"/>
-      <c r="R55" s="4"/>
-      <c r="S55" s="4"/>
-      <c r="T55" s="4"/>
-      <c r="U55" s="4"/>
-      <c r="V55" s="4"/>
-      <c r="W55" s="4"/>
-      <c r="X55" s="4"/>
-      <c r="Y55" s="4"/>
-      <c r="Z55" s="4"/>
-      <c r="AA55" s="4"/>
-    </row>
-    <row r="56" spans="1:27" ht="100.8">
-      <c r="A56" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E56" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="F56" s="4"/>
-      <c r="G56" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H56" s="6"/>
-      <c r="I56" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="4"/>
-      <c r="N56" s="4"/>
-      <c r="O56" s="4"/>
-      <c r="P56" s="4"/>
-      <c r="Q56" s="4"/>
-      <c r="R56" s="4"/>
-      <c r="S56" s="4"/>
-      <c r="T56" s="4"/>
-      <c r="U56" s="4"/>
-      <c r="V56" s="4"/>
-      <c r="W56" s="4"/>
-      <c r="X56" s="4"/>
-      <c r="Y56" s="4"/>
-      <c r="Z56" s="4"/>
-      <c r="AA56" s="4"/>
-    </row>
-    <row r="57" spans="1:27" ht="14.4">
-      <c r="A57" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="6"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
-      <c r="N57" s="4"/>
-      <c r="O57" s="4"/>
-      <c r="P57" s="4"/>
-      <c r="Q57" s="4"/>
-      <c r="R57" s="4"/>
-      <c r="S57" s="4"/>
-      <c r="T57" s="4"/>
-      <c r="U57" s="4"/>
-      <c r="V57" s="4"/>
-      <c r="W57" s="4"/>
-      <c r="X57" s="4"/>
-      <c r="Y57" s="4"/>
-      <c r="Z57" s="4"/>
-      <c r="AA57" s="4"/>
     </row>
     <row r="58" spans="1:27" ht="14.4">
       <c r="A58" s="5"/>
@@ -3135,16 +3042,28 @@
       <c r="Z59" s="4"/>
       <c r="AA59" s="4"/>
     </row>
-    <row r="60" spans="1:27" ht="14.4">
+    <row r="60" spans="1:27" ht="158.4">
       <c r="A60" s="5"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="6"/>
+      <c r="B60" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E60" s="25" t="s">
+        <v>104</v>
+      </c>
       <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
+      <c r="G60" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="H60" s="6"/>
-      <c r="I60" s="4"/>
+      <c r="I60" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
@@ -3164,16 +3083,30 @@
       <c r="Z60" s="4"/>
       <c r="AA60" s="4"/>
     </row>
-    <row r="61" spans="1:27" ht="14.4">
-      <c r="A61" s="5"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="6"/>
+    <row r="61" spans="1:27" ht="100.8">
+      <c r="A61" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E61" s="25" t="s">
+        <v>104</v>
+      </c>
       <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
+      <c r="G61" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="H61" s="6"/>
-      <c r="I61" s="4"/>
+      <c r="I61" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
@@ -3194,7 +3127,9 @@
       <c r="AA61" s="4"/>
     </row>
     <row r="62" spans="1:27" ht="14.4">
-      <c r="A62" s="5"/>
+      <c r="A62" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="B62" s="3"/>
       <c r="C62" s="6"/>
       <c r="D62" s="4"/>

</xml_diff>

<commit_message>
codebooks for templates 1-7 completed
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="170">
   <si>
     <t>release</t>
   </si>
@@ -330,19 +330,7 @@
     <t>D5_DU_matching_diagnostic</t>
   </si>
   <si>
-    <t>09_T3_10_match</t>
-  </si>
-  <si>
-    <t>D3_DU_MS-PREGNANCY-COHORT D3_DU_MS-COHORT</t>
-  </si>
-  <si>
-    <t>08_T3_30_create_prevalence_MS_in_pregnancy_cohort</t>
-  </si>
-  <si>
     <t>D3_DU_selection_criteria_from_SAP1_MS_cohort_to_DU_MS_cohort D3_SAP1_MS-COHORT</t>
-  </si>
-  <si>
-    <t>08_T4_40_create_templates_on_prevalence_MS_in_pregnancy_cohort</t>
   </si>
   <si>
     <t>numbers to be included in Template 1:  Description of the time period between 2 pregnancies in the pregnancy cohort and in the MS-pregnancy cohort</t>
@@ -472,26 +460,95 @@
     <t>08_T4_20_create_descriptives_pregnancies</t>
   </si>
   <si>
-    <t>D3_candidate_matches_MS_non_pregnant</t>
-  </si>
-  <si>
-    <t>09_create_candidate_matches_MS_non_pregnant</t>
-  </si>
-  <si>
     <t>contains the aggregated prevalence (numerators and denominators) needed to compute prevalence of MS in the pregnancy cohort, to feed Template 4 and 5</t>
   </si>
   <si>
-    <t xml:space="preserve">This applies some of the steps in the appendix: all the </t>
+    <t>Prevalence of MS over time per 1,000 pregnancies from women aged 15-49 years old</t>
   </si>
   <si>
-    <t>Prevalence of MS over time per 1,000 pregnancies from women aged 15-49 years old</t>
+    <t>D5_DU_for_Template_3</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">D3_DU_PREGNANCY-COHORT_variables </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>conceptsets</t>
+    </r>
+  </si>
+  <si>
+    <t>D4_DU_individual_prevalence_of_use_MSdrugs_in_MSpregnancy_cohort</t>
+  </si>
+  <si>
+    <t>D4_DU_prevalence_of_use_MSdrugs_in_MSpregnancy_cohort</t>
+  </si>
+  <si>
+    <t>Prevalence of MS stratified by age at LMP and calendar period per 1,000 pregnancies</t>
+  </si>
+  <si>
+    <t>Pattern of MS DMT medications1 use (for each drug individually and for any MS drug use) during pregnancy in women from the MS Pregnancy cohort</t>
+  </si>
+  <si>
+    <t>D4_DU_prevalence_of_use_MSdrugs_in_MS_cohort</t>
+  </si>
+  <si>
+    <t>contains the aggregated prevalence of use (numerators and denominators) needed to feed Template 6</t>
+  </si>
+  <si>
+    <t>D5_DU_for_Template_6</t>
+  </si>
+  <si>
+    <t>Prevalence of medication in women of childbearing age with MS at cohort entry over time</t>
+  </si>
+  <si>
+    <t>11_T4_30_create_template_on_prevalence_of_use_MSdrugs_in_MS_cohort</t>
+  </si>
+  <si>
+    <t>11_T4_20_create_templates_on_prevalence_MS_in_pregnancy_cohort</t>
+  </si>
+  <si>
+    <t>11_T4_10_create_template_on_prevalence_of_use_MSdrugs_in_MSpregnancy_cohort</t>
+  </si>
+  <si>
+    <t>10_T3_20_create_prevalence_of_use_MSdrugs_in_MS_cohort</t>
+  </si>
+  <si>
+    <t>10_T3_20_create_prevalence_of_use_MSdrugs_in_MSpregnancy_cohort</t>
+  </si>
+  <si>
+    <t>10_T3_10_create_prevalence_MS_in_pregnancy_cohort</t>
+  </si>
+  <si>
+    <t>09_T3_20_match</t>
+  </si>
+  <si>
+    <t>09_T3_10_create_candidate_matches_MS_non_pregnant</t>
+  </si>
+  <si>
+    <t>This applies some of the steps in the appendix: selects all the periods when women with MS are outside of the pregnancy cohort</t>
+  </si>
+  <si>
+    <t>D4_candidate_matches_MS_non_pregnant</t>
+  </si>
+  <si>
+    <t>D3_DU_MS-PREGNANCY-COHORT_variables D4_candidate_matches_MS_non_pregnant</t>
+  </si>
+  <si>
+    <t>D3_DU_PREGNANCY-COHORT_variables D4_DU_MS-COHORT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -561,6 +618,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -606,7 +676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -677,6 +747,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -895,20 +966,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA1040"/>
+  <dimension ref="A1:AA1045"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C46" sqref="C46"/>
+      <selection pane="bottomRight" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="6.44140625" customWidth="1"/>
     <col min="2" max="2" width="38.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" customWidth="1"/>
     <col min="4" max="4" width="48.77734375" customWidth="1"/>
     <col min="5" max="5" width="46" customWidth="1"/>
     <col min="7" max="7" width="28.33203125" customWidth="1"/>
@@ -1439,7 +1510,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>45</v>
@@ -1477,7 +1548,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>45</v>
@@ -1593,7 +1664,7 @@
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>48</v>
@@ -1632,7 +1703,7 @@
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="22" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>48</v>
@@ -1667,7 +1738,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>49</v>
@@ -1676,7 +1747,7 @@
         <v>50</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="9" t="s">
@@ -1714,10 +1785,10 @@
         <v>51</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="9" t="s">
@@ -2147,14 +2218,14 @@
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
       <c r="A32" s="28"/>
       <c r="B32" s="32" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="25" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="25"/>
@@ -2182,13 +2253,13 @@
     <row r="33" spans="1:27" ht="15.75" customHeight="1">
       <c r="A33" s="5"/>
       <c r="B33" s="25" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="25"/>
@@ -2216,14 +2287,14 @@
     <row r="34" spans="1:27" ht="15.75" customHeight="1">
       <c r="A34" s="5"/>
       <c r="B34" s="25" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C34" s="14"/>
       <c r="D34" s="25" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="25"/>
@@ -2251,13 +2322,13 @@
     <row r="35" spans="1:27" ht="15.75" customHeight="1">
       <c r="A35" s="5"/>
       <c r="B35" s="25" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="25"/>
@@ -2285,14 +2356,14 @@
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
       <c r="A36" s="5"/>
       <c r="B36" s="25" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="25" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="25"/>
@@ -2320,13 +2391,13 @@
     <row r="37" spans="1:27" ht="15.75" customHeight="1">
       <c r="A37" s="5"/>
       <c r="B37" s="25" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="25"/>
@@ -2354,14 +2425,14 @@
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
       <c r="A38" s="5"/>
       <c r="B38" s="25" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C38" s="14"/>
       <c r="D38" s="25" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="25"/>
@@ -2389,13 +2460,13 @@
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
       <c r="A39" s="5"/>
       <c r="B39" s="25" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="25"/>
@@ -2423,14 +2494,14 @@
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="32" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C40" s="14"/>
       <c r="D40" s="25" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="25"/>
@@ -2458,14 +2529,14 @@
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
       <c r="A41" s="5"/>
       <c r="B41" s="32" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="25" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="25"/>
@@ -2501,7 +2572,7 @@
         <v>68</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E42" s="24" t="s">
         <v>69</v>
@@ -2540,7 +2611,7 @@
         <v>71</v>
       </c>
       <c r="D43" s="33" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E43" s="39" t="s">
         <v>67</v>
@@ -2575,16 +2646,16 @@
         <v>66</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C44" s="40" t="s">
         <v>77</v>
       </c>
       <c r="D44" s="33" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E44" s="41" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F44" s="35"/>
       <c r="G44" s="4"/>
@@ -2616,16 +2687,16 @@
         <v>66</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C45" s="40" t="s">
         <v>73</v>
       </c>
       <c r="D45" s="33" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F45" s="35"/>
       <c r="G45" s="4"/>
@@ -2663,7 +2734,7 @@
         <v>75</v>
       </c>
       <c r="D46" s="33" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E46" s="32" t="s">
         <v>70</v>
@@ -2695,10 +2766,10 @@
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
       <c r="B47" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E47" s="25" t="s">
         <v>76</v>
@@ -2709,13 +2780,13 @@
         <v>66</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>79</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E48" s="25" t="s">
         <v>76</v>
@@ -2748,16 +2819,16 @@
         <v>66</v>
       </c>
       <c r="B49" s="33" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C49" s="34" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D49" s="33" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E49" s="32" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F49" s="35"/>
       <c r="G49" s="4"/>
@@ -2789,16 +2860,16 @@
         <v>66</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C50" s="36" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D50" s="33" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E50" s="33" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F50" s="35"/>
       <c r="G50" s="4"/>
@@ -2823,19 +2894,19 @@
       <c r="Z50" s="4"/>
       <c r="AA50" s="4"/>
     </row>
-    <row r="51" spans="1:27" ht="144">
+    <row r="51" spans="1:27" ht="72">
       <c r="A51" s="5"/>
       <c r="B51" s="33" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C51" s="36" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D51" s="33" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E51" s="33" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F51" s="35"/>
       <c r="G51" s="4"/>
@@ -2860,25 +2931,23 @@
       <c r="Z51" s="4"/>
       <c r="AA51" s="4"/>
     </row>
-    <row r="52" spans="1:27" ht="115.2">
+    <row r="52" spans="1:27" ht="43.2">
       <c r="A52" s="5"/>
       <c r="B52" s="3" t="s">
-        <v>80</v>
+        <v>167</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>105</v>
+        <v>165</v>
       </c>
-      <c r="E52" s="33" t="s">
-        <v>116</v>
+      <c r="E52" s="6" t="s">
+        <v>169</v>
       </c>
-      <c r="F52" s="4"/>
-      <c r="G52" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H52" s="6"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="15"/>
       <c r="I52" s="3"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
@@ -2899,24 +2968,22 @@
       <c r="Z52" s="4"/>
       <c r="AA52" s="4"/>
     </row>
-    <row r="53" spans="1:27" ht="14.4">
-      <c r="A53" s="5" t="s">
-        <v>66</v>
+    <row r="53" spans="1:27" ht="72">
+      <c r="A53" s="5"/>
+      <c r="B53" s="3" t="s">
+        <v>81</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C53" s="25" t="s">
-        <v>154</v>
+      <c r="C53" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>107</v>
+        <v>164</v>
       </c>
-      <c r="E53" s="3" t="s">
-        <v>80</v>
+      <c r="E53" s="25" t="s">
+        <v>168</v>
       </c>
-      <c r="F53" s="4"/>
-      <c r="G53" s="3"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="4"/>
       <c r="H53" s="15"/>
       <c r="I53" s="3"/>
       <c r="J53" s="4"/>
@@ -2938,20 +3005,22 @@
       <c r="Z53" s="4"/>
       <c r="AA53" s="4"/>
     </row>
-    <row r="54" spans="1:27" ht="14.4">
+    <row r="54" spans="1:27" ht="57.6">
       <c r="A54" s="5"/>
       <c r="B54" s="3" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
-      <c r="C54" s="15"/>
+      <c r="C54" s="15" t="s">
+        <v>83</v>
+      </c>
       <c r="D54" s="3" t="s">
-        <v>107</v>
+        <v>164</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>80</v>
+      <c r="E54" s="25" t="s">
+        <v>168</v>
       </c>
-      <c r="F54" s="4"/>
-      <c r="G54" s="3"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="4"/>
       <c r="H54" s="15"/>
       <c r="I54" s="3"/>
       <c r="J54" s="4"/>
@@ -2973,27 +3042,133 @@
       <c r="Z54" s="4"/>
       <c r="AA54" s="4"/>
     </row>
-    <row r="55" spans="1:27" ht="15.75" customHeight="1">
+    <row r="55" spans="1:27" ht="57.6">
+      <c r="A55" s="5"/>
       <c r="B55" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E55" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="F55" s="4"/>
+      <c r="G55" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H55" s="6"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
+      <c r="S55" s="4"/>
+      <c r="T55" s="4"/>
+      <c r="U55" s="4"/>
+      <c r="V55" s="4"/>
+      <c r="W55" s="4"/>
+      <c r="X55" s="4"/>
+      <c r="Y55" s="4"/>
+      <c r="Z55" s="4"/>
+      <c r="AA55" s="4"/>
+    </row>
+    <row r="56" spans="1:27" ht="43.2">
+      <c r="A56" s="5"/>
+      <c r="B56" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E56" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="F56" s="4"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4"/>
+      <c r="T56" s="4"/>
+      <c r="U56" s="4"/>
+      <c r="V56" s="4"/>
+      <c r="W56" s="4"/>
+      <c r="X56" s="4"/>
+      <c r="Y56" s="4"/>
+      <c r="Z56" s="4"/>
+      <c r="AA56" s="4"/>
+    </row>
+    <row r="57" spans="1:27" ht="14.4">
+      <c r="A57" s="5"/>
+      <c r="B57" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C57" s="15"/>
+      <c r="D57" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E57" s="33"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+      <c r="U57" s="4"/>
+      <c r="V57" s="4"/>
+      <c r="W57" s="4"/>
+      <c r="X57" s="4"/>
+      <c r="Y57" s="4"/>
+      <c r="Z57" s="4"/>
+      <c r="AA57" s="4"/>
+    </row>
+    <row r="58" spans="1:27" ht="57.6">
+      <c r="A58" s="5"/>
+      <c r="B58" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C55" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="58" spans="1:27" ht="14.4">
-      <c r="A58" s="5"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="6"/>
       <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="6"/>
-      <c r="I58" s="4"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="3"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
@@ -3014,15 +3189,25 @@
       <c r="AA58" s="4"/>
     </row>
     <row r="59" spans="1:27" ht="14.4">
-      <c r="A59" s="5"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="6"/>
+      <c r="A59" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="6"/>
-      <c r="I59" s="4"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="3"/>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
@@ -3042,28 +3227,24 @@
       <c r="Z59" s="4"/>
       <c r="AA59" s="4"/>
     </row>
-    <row r="60" spans="1:27" ht="158.4">
+    <row r="60" spans="1:27" ht="14.4">
       <c r="A60" s="5"/>
       <c r="B60" s="3" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
-      <c r="C60" s="15" t="s">
-        <v>82</v>
+      <c r="C60" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>103</v>
+        <v>159</v>
       </c>
-      <c r="E60" s="25" t="s">
-        <v>104</v>
+      <c r="E60" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="F60" s="4"/>
-      <c r="G60" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H60" s="6"/>
-      <c r="I60" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="G60" s="3"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="3"/>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
@@ -3083,30 +3264,24 @@
       <c r="Z60" s="4"/>
       <c r="AA60" s="4"/>
     </row>
-    <row r="61" spans="1:27" ht="100.8">
-      <c r="A61" s="5" t="s">
-        <v>66</v>
+    <row r="61" spans="1:27" ht="14.4">
+      <c r="A61" s="5"/>
+      <c r="B61" s="3" t="s">
+        <v>156</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>83</v>
+      <c r="C61" s="42" t="s">
+        <v>157</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>103</v>
+        <v>158</v>
       </c>
-      <c r="E61" s="25" t="s">
-        <v>104</v>
+      <c r="E61" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="F61" s="4"/>
-      <c r="G61" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H61" s="6"/>
-      <c r="I61" s="3" t="s">
-        <v>84</v>
-      </c>
+      <c r="G61" s="3"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="3"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
@@ -3127,17 +3302,15 @@
       <c r="AA61" s="4"/>
     </row>
     <row r="62" spans="1:27" ht="14.4">
-      <c r="A62" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="A62" s="5"/>
       <c r="B62" s="3"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="6"/>
+      <c r="C62" s="42"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
       <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="6"/>
-      <c r="I62" s="4"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="3"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
@@ -3158,15 +3331,15 @@
       <c r="AA62" s="4"/>
     </row>
     <row r="63" spans="1:27" ht="14.4">
-      <c r="A63" s="6"/>
+      <c r="A63" s="5"/>
       <c r="B63" s="3"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="6"/>
+      <c r="C63" s="42"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
       <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="6"/>
-      <c r="I63" s="4"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="3"/>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
@@ -3187,11 +3360,7 @@
       <c r="AA63" s="4"/>
     </row>
     <row r="64" spans="1:27" ht="14.4">
-      <c r="A64" s="6"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="6"/>
+      <c r="A64" s="5"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
       <c r="H64" s="6"/>
@@ -3216,15 +3385,11 @@
       <c r="AA64" s="4"/>
     </row>
     <row r="65" spans="1:27" ht="14.4">
-      <c r="A65" s="6"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="6"/>
+      <c r="A65" s="5"/>
       <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
+      <c r="G65" s="3"/>
       <c r="H65" s="6"/>
-      <c r="I65" s="4"/>
+      <c r="I65" s="3"/>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
       <c r="L65" s="4"/>
@@ -3245,15 +3410,17 @@
       <c r="AA65" s="4"/>
     </row>
     <row r="66" spans="1:27" ht="14.4">
-      <c r="A66" s="6"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="6"/>
+      <c r="A66" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
+      <c r="G66" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="H66" s="6"/>
-      <c r="I66" s="4"/>
+      <c r="I66" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
@@ -3274,7 +3441,7 @@
       <c r="AA66" s="4"/>
     </row>
     <row r="67" spans="1:27" ht="14.4">
-      <c r="A67" s="6"/>
+      <c r="A67" s="5"/>
       <c r="B67" s="3"/>
       <c r="C67" s="6"/>
       <c r="D67" s="4"/>
@@ -31490,8 +31657,153 @@
       <c r="Z1039" s="4"/>
       <c r="AA1039" s="4"/>
     </row>
-    <row r="1040" spans="1:27" ht="15.75" customHeight="1">
+    <row r="1040" spans="1:27" ht="14.4">
       <c r="A1040" s="6"/>
+      <c r="B1040" s="3"/>
+      <c r="C1040" s="6"/>
+      <c r="D1040" s="4"/>
+      <c r="E1040" s="6"/>
+      <c r="F1040" s="4"/>
+      <c r="G1040" s="4"/>
+      <c r="H1040" s="6"/>
+      <c r="I1040" s="4"/>
+      <c r="J1040" s="4"/>
+      <c r="K1040" s="4"/>
+      <c r="L1040" s="4"/>
+      <c r="M1040" s="4"/>
+      <c r="N1040" s="4"/>
+      <c r="O1040" s="4"/>
+      <c r="P1040" s="4"/>
+      <c r="Q1040" s="4"/>
+      <c r="R1040" s="4"/>
+      <c r="S1040" s="4"/>
+      <c r="T1040" s="4"/>
+      <c r="U1040" s="4"/>
+      <c r="V1040" s="4"/>
+      <c r="W1040" s="4"/>
+      <c r="X1040" s="4"/>
+      <c r="Y1040" s="4"/>
+      <c r="Z1040" s="4"/>
+      <c r="AA1040" s="4"/>
+    </row>
+    <row r="1041" spans="1:27" ht="14.4">
+      <c r="A1041" s="6"/>
+      <c r="B1041" s="3"/>
+      <c r="C1041" s="6"/>
+      <c r="D1041" s="4"/>
+      <c r="E1041" s="6"/>
+      <c r="F1041" s="4"/>
+      <c r="G1041" s="4"/>
+      <c r="H1041" s="6"/>
+      <c r="I1041" s="4"/>
+      <c r="J1041" s="4"/>
+      <c r="K1041" s="4"/>
+      <c r="L1041" s="4"/>
+      <c r="M1041" s="4"/>
+      <c r="N1041" s="4"/>
+      <c r="O1041" s="4"/>
+      <c r="P1041" s="4"/>
+      <c r="Q1041" s="4"/>
+      <c r="R1041" s="4"/>
+      <c r="S1041" s="4"/>
+      <c r="T1041" s="4"/>
+      <c r="U1041" s="4"/>
+      <c r="V1041" s="4"/>
+      <c r="W1041" s="4"/>
+      <c r="X1041" s="4"/>
+      <c r="Y1041" s="4"/>
+      <c r="Z1041" s="4"/>
+      <c r="AA1041" s="4"/>
+    </row>
+    <row r="1042" spans="1:27" ht="14.4">
+      <c r="A1042" s="6"/>
+      <c r="B1042" s="3"/>
+      <c r="C1042" s="6"/>
+      <c r="D1042" s="4"/>
+      <c r="E1042" s="6"/>
+      <c r="F1042" s="4"/>
+      <c r="G1042" s="4"/>
+      <c r="H1042" s="6"/>
+      <c r="I1042" s="4"/>
+      <c r="J1042" s="4"/>
+      <c r="K1042" s="4"/>
+      <c r="L1042" s="4"/>
+      <c r="M1042" s="4"/>
+      <c r="N1042" s="4"/>
+      <c r="O1042" s="4"/>
+      <c r="P1042" s="4"/>
+      <c r="Q1042" s="4"/>
+      <c r="R1042" s="4"/>
+      <c r="S1042" s="4"/>
+      <c r="T1042" s="4"/>
+      <c r="U1042" s="4"/>
+      <c r="V1042" s="4"/>
+      <c r="W1042" s="4"/>
+      <c r="X1042" s="4"/>
+      <c r="Y1042" s="4"/>
+      <c r="Z1042" s="4"/>
+      <c r="AA1042" s="4"/>
+    </row>
+    <row r="1043" spans="1:27" ht="14.4">
+      <c r="A1043" s="6"/>
+      <c r="B1043" s="3"/>
+      <c r="C1043" s="6"/>
+      <c r="D1043" s="4"/>
+      <c r="E1043" s="6"/>
+      <c r="F1043" s="4"/>
+      <c r="G1043" s="4"/>
+      <c r="H1043" s="6"/>
+      <c r="I1043" s="4"/>
+      <c r="J1043" s="4"/>
+      <c r="K1043" s="4"/>
+      <c r="L1043" s="4"/>
+      <c r="M1043" s="4"/>
+      <c r="N1043" s="4"/>
+      <c r="O1043" s="4"/>
+      <c r="P1043" s="4"/>
+      <c r="Q1043" s="4"/>
+      <c r="R1043" s="4"/>
+      <c r="S1043" s="4"/>
+      <c r="T1043" s="4"/>
+      <c r="U1043" s="4"/>
+      <c r="V1043" s="4"/>
+      <c r="W1043" s="4"/>
+      <c r="X1043" s="4"/>
+      <c r="Y1043" s="4"/>
+      <c r="Z1043" s="4"/>
+      <c r="AA1043" s="4"/>
+    </row>
+    <row r="1044" spans="1:27" ht="14.4">
+      <c r="A1044" s="6"/>
+      <c r="B1044" s="3"/>
+      <c r="C1044" s="6"/>
+      <c r="D1044" s="4"/>
+      <c r="E1044" s="6"/>
+      <c r="F1044" s="4"/>
+      <c r="G1044" s="4"/>
+      <c r="H1044" s="6"/>
+      <c r="I1044" s="4"/>
+      <c r="J1044" s="4"/>
+      <c r="K1044" s="4"/>
+      <c r="L1044" s="4"/>
+      <c r="M1044" s="4"/>
+      <c r="N1044" s="4"/>
+      <c r="O1044" s="4"/>
+      <c r="P1044" s="4"/>
+      <c r="Q1044" s="4"/>
+      <c r="R1044" s="4"/>
+      <c r="S1044" s="4"/>
+      <c r="T1044" s="4"/>
+      <c r="U1044" s="4"/>
+      <c r="V1044" s="4"/>
+      <c r="W1044" s="4"/>
+      <c r="X1044" s="4"/>
+      <c r="Y1044" s="4"/>
+      <c r="Z1044" s="4"/>
+      <c r="AA1044" s="4"/>
+    </row>
+    <row r="1045" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A1045" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
codebooks for matched non-pregnant MS
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="168">
   <si>
     <t>release</t>
   </si>
@@ -273,9 +273,6 @@
     <t>contains the success rate of matching (to be refined after the matching function is finalised), per relevant covariates (including quality of pregnancy)</t>
   </si>
   <si>
-    <t>to be created by R&amp;D, remember to add quality of pregnancies</t>
-  </si>
-  <si>
     <t>slug</t>
   </si>
   <si>
@@ -469,21 +466,6 @@
     <t>D5_DU_for_Template_3</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">D3_DU_PREGNANCY-COHORT_variables </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>conceptsets</t>
-    </r>
-  </si>
-  <si>
     <t>D4_DU_individual_prevalence_of_use_MSdrugs_in_MSpregnancy_cohort</t>
   </si>
   <si>
@@ -548,7 +530,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -617,13 +599,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -747,7 +722,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -966,13 +941,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA1045"/>
+  <dimension ref="A1:AA1044"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C52" sqref="C52"/>
+      <selection pane="bottomRight" activeCell="A66" sqref="A66:XFD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1015,7 +990,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -1510,7 +1485,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>45</v>
@@ -1548,7 +1523,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>45</v>
@@ -1660,11 +1635,11 @@
         <v>9</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>48</v>
@@ -1699,11 +1674,11 @@
         <v>9</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>48</v>
@@ -1738,7 +1713,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>49</v>
@@ -1747,7 +1722,7 @@
         <v>50</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="9" t="s">
@@ -1779,16 +1754,16 @@
         <v>9</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="9" t="s">
@@ -1820,7 +1795,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>52</v>
@@ -1861,7 +1836,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="3" t="s">
@@ -1900,7 +1875,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>55</v>
@@ -1941,7 +1916,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="3" t="s">
@@ -1980,7 +1955,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>57</v>
@@ -2021,7 +1996,7 @@
         <v>9</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="3" t="s">
@@ -2060,16 +2035,16 @@
         <v>9</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>59</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="9" t="s">
@@ -2101,16 +2076,16 @@
         <v>9</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>59</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="9" t="s">
@@ -2142,7 +2117,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>60</v>
@@ -2151,7 +2126,7 @@
         <v>61</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="9" t="s">
@@ -2181,16 +2156,16 @@
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
       <c r="A31" s="5"/>
       <c r="B31" s="32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D31" s="25" t="s">
         <v>61</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="25"/>
@@ -2218,14 +2193,14 @@
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
       <c r="A32" s="28"/>
       <c r="B32" s="32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="25"/>
@@ -2253,13 +2228,13 @@
     <row r="33" spans="1:27" ht="15.75" customHeight="1">
       <c r="A33" s="5"/>
       <c r="B33" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="25"/>
@@ -2287,14 +2262,14 @@
     <row r="34" spans="1:27" ht="15.75" customHeight="1">
       <c r="A34" s="5"/>
       <c r="B34" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C34" s="14"/>
       <c r="D34" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="25"/>
@@ -2322,13 +2297,13 @@
     <row r="35" spans="1:27" ht="15.75" customHeight="1">
       <c r="A35" s="5"/>
       <c r="B35" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="25"/>
@@ -2356,14 +2331,14 @@
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
       <c r="A36" s="5"/>
       <c r="B36" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="25"/>
@@ -2391,13 +2366,13 @@
     <row r="37" spans="1:27" ht="15.75" customHeight="1">
       <c r="A37" s="5"/>
       <c r="B37" s="25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="25"/>
@@ -2425,14 +2400,14 @@
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
       <c r="A38" s="5"/>
       <c r="B38" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C38" s="14"/>
       <c r="D38" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="25"/>
@@ -2460,13 +2435,13 @@
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
       <c r="A39" s="5"/>
       <c r="B39" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="25"/>
@@ -2494,14 +2469,14 @@
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C40" s="14"/>
       <c r="D40" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="25"/>
@@ -2529,14 +2504,14 @@
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
       <c r="A41" s="5"/>
       <c r="B41" s="32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="25"/>
@@ -2561,7 +2536,7 @@
       <c r="Z41" s="4"/>
       <c r="AA41" s="4"/>
     </row>
-    <row r="42" spans="1:27" ht="72">
+    <row r="42" spans="1:27" ht="43.2">
       <c r="A42" s="5" t="s">
         <v>66</v>
       </c>
@@ -2572,7 +2547,7 @@
         <v>68</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E42" s="24" t="s">
         <v>69</v>
@@ -2600,7 +2575,7 @@
       <c r="Z42" s="4"/>
       <c r="AA42" s="4"/>
     </row>
-    <row r="43" spans="1:27" ht="86.4">
+    <row r="43" spans="1:27" ht="43.2">
       <c r="A43" s="5" t="s">
         <v>66</v>
       </c>
@@ -2611,7 +2586,7 @@
         <v>71</v>
       </c>
       <c r="D43" s="33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E43" s="39" t="s">
         <v>67</v>
@@ -2641,21 +2616,21 @@
       <c r="Z43" s="4"/>
       <c r="AA43" s="4"/>
     </row>
-    <row r="44" spans="1:27" ht="100.8">
+    <row r="44" spans="1:27" ht="57.6">
       <c r="A44" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C44" s="40" t="s">
         <v>77</v>
       </c>
       <c r="D44" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E44" s="41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F44" s="35"/>
       <c r="G44" s="4"/>
@@ -2682,21 +2657,21 @@
       <c r="Z44" s="4"/>
       <c r="AA44" s="4"/>
     </row>
-    <row r="45" spans="1:27" ht="57.6">
+    <row r="45" spans="1:27" ht="28.8">
       <c r="A45" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C45" s="40" t="s">
         <v>73</v>
       </c>
       <c r="D45" s="33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F45" s="35"/>
       <c r="G45" s="4"/>
@@ -2723,7 +2698,7 @@
       <c r="Z45" s="4"/>
       <c r="AA45" s="4"/>
     </row>
-    <row r="46" spans="1:27" ht="43.2">
+    <row r="46" spans="1:27" ht="28.8">
       <c r="A46" s="5" t="s">
         <v>66</v>
       </c>
@@ -2734,7 +2709,7 @@
         <v>75</v>
       </c>
       <c r="D46" s="33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E46" s="32" t="s">
         <v>70</v>
@@ -2766,27 +2741,27 @@
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
       <c r="B47" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E47" s="25" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="43.2">
+    <row r="48" spans="1:27" ht="28.8">
       <c r="A48" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>79</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E48" s="25" t="s">
         <v>76</v>
@@ -2819,16 +2794,16 @@
         <v>66</v>
       </c>
       <c r="B49" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C49" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D49" s="33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E49" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F49" s="35"/>
       <c r="G49" s="4"/>
@@ -2855,21 +2830,21 @@
       <c r="Z49" s="4"/>
       <c r="AA49" s="4"/>
     </row>
-    <row r="50" spans="1:27" ht="115.2">
+    <row r="50" spans="1:27" ht="57.6">
       <c r="A50" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C50" s="36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D50" s="33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E50" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F50" s="35"/>
       <c r="G50" s="4"/>
@@ -2897,16 +2872,16 @@
     <row r="51" spans="1:27" ht="72">
       <c r="A51" s="5"/>
       <c r="B51" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C51" s="36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D51" s="33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E51" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F51" s="35"/>
       <c r="G51" s="4"/>
@@ -2934,16 +2909,16 @@
     <row r="52" spans="1:27" ht="43.2">
       <c r="A52" s="5"/>
       <c r="B52" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F52" s="35"/>
       <c r="G52" s="4"/>
@@ -2977,10 +2952,10 @@
         <v>82</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E53" s="25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F53" s="35"/>
       <c r="G53" s="4"/>
@@ -3008,16 +2983,16 @@
     <row r="54" spans="1:27" ht="57.6">
       <c r="A54" s="5"/>
       <c r="B54" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>83</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E54" s="25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F54" s="35"/>
       <c r="G54" s="4"/>
@@ -3048,13 +3023,13 @@
         <v>80</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E55" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="3" t="s">
@@ -3084,16 +3059,16 @@
     <row r="56" spans="1:27" ht="43.2">
       <c r="A56" s="5"/>
       <c r="B56" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E56" s="33" t="s">
-        <v>149</v>
+        <v>81</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="3"/>
@@ -3121,13 +3096,15 @@
     <row r="57" spans="1:27" ht="14.4">
       <c r="A57" s="5"/>
       <c r="B57" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C57" s="15"/>
       <c r="D57" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
-      <c r="E57" s="33"/>
+      <c r="E57" s="33" t="s">
+        <v>81</v>
+      </c>
       <c r="F57" s="4"/>
       <c r="G57" s="3"/>
       <c r="H57" s="15"/>
@@ -3154,16 +3131,16 @@
     <row r="58" spans="1:27" ht="57.6">
       <c r="A58" s="5"/>
       <c r="B58" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="3"/>
@@ -3193,13 +3170,13 @@
         <v>66</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>80</v>
@@ -3230,13 +3207,13 @@
     <row r="60" spans="1:27" ht="14.4">
       <c r="A60" s="5"/>
       <c r="B60" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C60" s="42" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>80</v>
@@ -3267,16 +3244,16 @@
     <row r="61" spans="1:27" ht="14.4">
       <c r="A61" s="5"/>
       <c r="B61" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C61" s="42" t="s">
-        <v>157</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="E61" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F61" s="4"/>
       <c r="G61" s="3"/>
@@ -3410,17 +3387,15 @@
       <c r="AA65" s="4"/>
     </row>
     <row r="66" spans="1:27" ht="14.4">
-      <c r="A66" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="A66" s="5"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="6"/>
       <c r="F66" s="4"/>
-      <c r="G66" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="G66" s="4"/>
       <c r="H66" s="6"/>
-      <c r="I66" s="3" t="s">
-        <v>84</v>
-      </c>
+      <c r="I66" s="4"/>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
@@ -3441,7 +3416,7 @@
       <c r="AA66" s="4"/>
     </row>
     <row r="67" spans="1:27" ht="14.4">
-      <c r="A67" s="5"/>
+      <c r="A67" s="6"/>
       <c r="B67" s="3"/>
       <c r="C67" s="6"/>
       <c r="D67" s="4"/>
@@ -31773,37 +31748,8 @@
       <c r="Z1043" s="4"/>
       <c r="AA1043" s="4"/>
     </row>
-    <row r="1044" spans="1:27" ht="14.4">
+    <row r="1044" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1044" s="6"/>
-      <c r="B1044" s="3"/>
-      <c r="C1044" s="6"/>
-      <c r="D1044" s="4"/>
-      <c r="E1044" s="6"/>
-      <c r="F1044" s="4"/>
-      <c r="G1044" s="4"/>
-      <c r="H1044" s="6"/>
-      <c r="I1044" s="4"/>
-      <c r="J1044" s="4"/>
-      <c r="K1044" s="4"/>
-      <c r="L1044" s="4"/>
-      <c r="M1044" s="4"/>
-      <c r="N1044" s="4"/>
-      <c r="O1044" s="4"/>
-      <c r="P1044" s="4"/>
-      <c r="Q1044" s="4"/>
-      <c r="R1044" s="4"/>
-      <c r="S1044" s="4"/>
-      <c r="T1044" s="4"/>
-      <c r="U1044" s="4"/>
-      <c r="V1044" s="4"/>
-      <c r="W1044" s="4"/>
-      <c r="X1044" s="4"/>
-      <c r="Y1044" s="4"/>
-      <c r="Z1044" s="4"/>
-      <c r="AA1044" s="4"/>
-    </row>
-    <row r="1045" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A1045" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
codebooks for templates 8-11
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="180">
   <si>
     <t>release</t>
   </si>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>D5_meaning_occurences with masked counts</t>
-  </si>
-  <si>
-    <t>not included yet</t>
   </si>
   <si>
     <t>D3_SAP1_MS-COHORT</t>
@@ -487,12 +484,6 @@
     <t>11_T4_10_create_template_on_prevalence_of_use_MSdrugs_in_MSpregnancy_cohort</t>
   </si>
   <si>
-    <t>10_T3_20_create_prevalence_of_use_MSdrugs_in_MS_cohort</t>
-  </si>
-  <si>
-    <t>10_T3_20_create_prevalence_of_use_MSdrugs_in_MSpregnancy_cohort</t>
-  </si>
-  <si>
     <t>10_T3_10_create_prevalence_MS_in_pregnancy_cohort</t>
   </si>
   <si>
@@ -526,20 +517,56 @@
     <t>Pattern of MS DMT medications use (for each drug individually and for any MS drug use) during pregnancy in women from the MS Pregnancy cohort</t>
   </si>
   <si>
-    <t>contains the aggregated prevalence of use (numerators and denominators) needed to feed Template 3</t>
-  </si>
-  <si>
     <t>Prevalence of MS medication in women of childbearing age with MS at cohort entry over time</t>
   </si>
   <si>
     <t>Prevalence of MS medication in women of childbearing age with MS at cohort entry by study period and age group</t>
+  </si>
+  <si>
+    <t>D4_DU_prevalence_of_exclusive_use_MSmeds_in_MSpregnancy_trimesters</t>
+  </si>
+  <si>
+    <t>10_T3_20_create_prevalence_of_exclusive_use_MSmeds_in_MSpregnancy_trimesters</t>
+  </si>
+  <si>
+    <t>D3_DU_PREGNANCY-COHORT_variables conceptsets</t>
+  </si>
+  <si>
+    <t>D4_DU_individual_prevalence_of_use_MSmeds_in_MSpregnancy_trimesters</t>
+  </si>
+  <si>
+    <t>10_T3_40_create_prevalence_of_use_MSdrugs_in_MSpregnancy_cohort</t>
+  </si>
+  <si>
+    <t>10_T3_30_create_prevalence_of_use_MSdrugs_in_MScohort</t>
+  </si>
+  <si>
+    <t>D4_DU_MS-COHORT conceptsets</t>
+  </si>
+  <si>
+    <t>contains the aggregated prevalence of use (numerators and denominators) needed to feed Templates 8+</t>
+  </si>
+  <si>
+    <t>this is the aggregation of the individual-level dataset D4_DU_individual_prevalence_of_use_MSmeds_in_MSpregnancy_trimesters, to feed Template 3. It copntains counts of persons using medicines exclusively in some periods before and during pregnancy</t>
+  </si>
+  <si>
+    <t>this dataset measures in each MS pregnancy whether the woman  used or didn't use each of the MS medications in the trimesters before or during pregnancy (to ultimately  feed Template 3)</t>
+  </si>
+  <si>
+    <t>D5_DU_for_Templats_8-11</t>
+  </si>
+  <si>
+    <t>numbers to be included in Templates 8-11, that explore use of medications in pregnant and matchd non-pregnant women with MS, across calendar period, ageband, pregnancy period</t>
+  </si>
+  <si>
+    <t>11_T4_30_create_template_on_prevalence_of_use_MSdrugs_in_MSpregnancy_cohort</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -615,8 +642,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -647,6 +680,18 @@
         <bgColor rgb="FF6AA84F"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -660,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -744,6 +789,14 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -963,19 +1016,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA1044"/>
+  <dimension ref="A1:AA1046"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C55" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E56" sqref="E56"/>
+      <selection pane="bottomRight" activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="6.44140625" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="64.88671875" customWidth="1"/>
     <col min="3" max="3" width="40.33203125" style="41" customWidth="1"/>
     <col min="4" max="4" width="48.77734375" customWidth="1"/>
     <col min="5" max="5" width="46" customWidth="1"/>
@@ -1012,7 +1065,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -1507,7 +1560,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>45</v>
@@ -1545,7 +1598,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>45</v>
@@ -1657,11 +1710,11 @@
         <v>9</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>48</v>
@@ -1696,11 +1749,11 @@
         <v>9</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>48</v>
@@ -1735,7 +1788,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>49</v>
@@ -1744,7 +1797,7 @@
         <v>50</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="9" t="s">
@@ -1776,16 +1829,16 @@
         <v>9</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="9" t="s">
@@ -1817,7 +1870,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>52</v>
@@ -1826,7 +1879,7 @@
         <v>53</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="9" t="s">
@@ -1858,14 +1911,14 @@
         <v>9</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="3" t="s">
         <v>53</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="9" t="s">
@@ -1897,7 +1950,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>55</v>
@@ -1906,7 +1959,7 @@
         <v>56</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="9" t="s">
@@ -1938,14 +1991,14 @@
         <v>9</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="9" t="s">
@@ -1977,7 +2030,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>57</v>
@@ -1986,7 +2039,7 @@
         <v>58</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="9" t="s">
@@ -2018,14 +2071,14 @@
         <v>9</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="9" t="s">
@@ -2057,16 +2110,16 @@
         <v>9</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>59</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="9" t="s">
@@ -2098,16 +2151,16 @@
         <v>9</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>59</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="9" t="s">
@@ -2139,7 +2192,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>60</v>
@@ -2148,7 +2201,7 @@
         <v>61</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="9" t="s">
@@ -2178,16 +2231,16 @@
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
       <c r="A31" s="5"/>
       <c r="B31" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D31" s="25" t="s">
         <v>61</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="25"/>
@@ -2215,14 +2268,14 @@
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
       <c r="A32" s="28"/>
       <c r="B32" s="32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="25"/>
@@ -2250,13 +2303,13 @@
     <row r="33" spans="1:27" ht="15.75" customHeight="1">
       <c r="A33" s="5"/>
       <c r="B33" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="25"/>
@@ -2284,14 +2337,14 @@
     <row r="34" spans="1:27" ht="15.75" customHeight="1">
       <c r="A34" s="5"/>
       <c r="B34" s="25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C34" s="14"/>
       <c r="D34" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="25"/>
@@ -2319,13 +2372,13 @@
     <row r="35" spans="1:27" ht="15.75" customHeight="1">
       <c r="A35" s="5"/>
       <c r="B35" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="25"/>
@@ -2353,14 +2406,14 @@
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
       <c r="A36" s="5"/>
       <c r="B36" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="25"/>
@@ -2388,13 +2441,13 @@
     <row r="37" spans="1:27" ht="15.75" customHeight="1">
       <c r="A37" s="5"/>
       <c r="B37" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="25"/>
@@ -2422,14 +2475,14 @@
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
       <c r="A38" s="5"/>
       <c r="B38" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C38" s="14"/>
       <c r="D38" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="25"/>
@@ -2457,13 +2510,13 @@
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
       <c r="A39" s="5"/>
       <c r="B39" s="25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="25"/>
@@ -2491,14 +2544,14 @@
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C40" s="14"/>
       <c r="D40" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="25"/>
@@ -2526,14 +2579,14 @@
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
       <c r="A41" s="5"/>
       <c r="B41" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="25"/>
@@ -2559,20 +2612,18 @@
       <c r="AA41" s="4"/>
     </row>
     <row r="42" spans="1:27" ht="43.2">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="46"/>
+      <c r="B42" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="C42" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C42" s="14" t="s">
-        <v>68</v>
-      </c>
       <c r="D42" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E42" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -2598,26 +2649,24 @@
       <c r="AA42" s="4"/>
     </row>
     <row r="43" spans="1:27" ht="43.2">
-      <c r="A43" s="5" t="s">
-        <v>66</v>
+      <c r="A43" s="46"/>
+      <c r="B43" s="36" t="s">
+        <v>69</v>
       </c>
-      <c r="B43" s="36" t="s">
+      <c r="C43" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="37" t="s">
-        <v>71</v>
-      </c>
       <c r="D43" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E43" s="38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F43" s="34"/>
       <c r="G43" s="4"/>
       <c r="H43" s="6"/>
       <c r="I43" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -2639,26 +2688,24 @@
       <c r="AA43" s="4"/>
     </row>
     <row r="44" spans="1:27" ht="57.6">
-      <c r="A44" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="A44" s="46"/>
       <c r="B44" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C44" s="39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D44" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E44" s="40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F44" s="34"/>
       <c r="G44" s="4"/>
       <c r="H44" s="6"/>
       <c r="I44" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -2680,26 +2727,24 @@
       <c r="AA44" s="4"/>
     </row>
     <row r="45" spans="1:27" ht="28.8">
-      <c r="A45" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="A45" s="46"/>
       <c r="B45" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C45" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D45" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F45" s="34"/>
       <c r="G45" s="4"/>
       <c r="H45" s="6"/>
       <c r="I45" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -2721,26 +2766,24 @@
       <c r="AA45" s="4"/>
     </row>
     <row r="46" spans="1:27" ht="28.8">
-      <c r="A46" s="5" t="s">
-        <v>66</v>
+      <c r="A46" s="46"/>
+      <c r="B46" s="33" t="s">
+        <v>73</v>
       </c>
-      <c r="B46" s="33" t="s">
+      <c r="C46" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="39" t="s">
-        <v>75</v>
-      </c>
       <c r="D46" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E46" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F46" s="34"/>
       <c r="G46" s="4"/>
       <c r="H46" s="6"/>
       <c r="I46" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
@@ -2762,31 +2805,30 @@
       <c r="AA46" s="4"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A47" s="47"/>
       <c r="B47" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:27" ht="28.8">
-      <c r="A48" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="A48" s="46"/>
       <c r="B48" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -2812,26 +2854,24 @@
       <c r="AA48" s="4"/>
     </row>
     <row r="49" spans="1:27" ht="27">
-      <c r="A49" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="A49" s="46"/>
       <c r="B49" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C49" s="43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D49" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E49" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F49" s="34"/>
       <c r="G49" s="4"/>
       <c r="H49" s="6"/>
       <c r="I49" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
@@ -2853,20 +2893,18 @@
       <c r="AA49" s="4"/>
     </row>
     <row r="50" spans="1:27" ht="57.6">
-      <c r="A50" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="A50" s="46"/>
       <c r="B50" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C50" s="35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D50" s="33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E50" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F50" s="34"/>
       <c r="G50" s="4"/>
@@ -2892,18 +2930,18 @@
       <c r="AA50" s="4"/>
     </row>
     <row r="51" spans="1:27" ht="72">
-      <c r="A51" s="5"/>
+      <c r="A51" s="46"/>
       <c r="B51" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C51" s="35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D51" s="33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E51" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F51" s="34"/>
       <c r="G51" s="4"/>
@@ -2929,18 +2967,18 @@
       <c r="AA51" s="4"/>
     </row>
     <row r="52" spans="1:27" ht="43.2">
-      <c r="A52" s="5"/>
+      <c r="A52" s="46"/>
       <c r="B52" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F52" s="34"/>
       <c r="G52" s="4"/>
@@ -2966,18 +3004,18 @@
       <c r="AA52" s="4"/>
     </row>
     <row r="53" spans="1:27" ht="72">
-      <c r="A53" s="5"/>
+      <c r="A53" s="46"/>
       <c r="B53" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C53" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C53" s="15" t="s">
-        <v>82</v>
-      </c>
       <c r="D53" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E53" s="25" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F53" s="34"/>
       <c r="G53" s="4"/>
@@ -3003,18 +3041,18 @@
       <c r="AA53" s="4"/>
     </row>
     <row r="54" spans="1:27" ht="57.6">
-      <c r="A54" s="5"/>
+      <c r="A54" s="46"/>
       <c r="B54" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E54" s="25" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F54" s="34"/>
       <c r="G54" s="4"/>
@@ -3040,18 +3078,18 @@
       <c r="AA54" s="4"/>
     </row>
     <row r="55" spans="1:27" ht="57.6">
-      <c r="A55" s="5"/>
+      <c r="A55" s="46"/>
       <c r="B55" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E55" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="3" t="s">
@@ -3078,19 +3116,19 @@
       <c r="Z55" s="4"/>
       <c r="AA55" s="4"/>
     </row>
-    <row r="56" spans="1:27" ht="43.2">
-      <c r="A56" s="5"/>
+    <row r="56" spans="1:27" ht="93.6">
+      <c r="A56" s="46"/>
       <c r="B56" s="3" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C56" s="49" t="s">
+        <v>176</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="E56" s="33" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="3"/>
@@ -3115,19 +3153,19 @@
       <c r="Z56" s="4"/>
       <c r="AA56" s="4"/>
     </row>
-    <row r="57" spans="1:27" ht="42" customHeight="1">
-      <c r="A57" s="5"/>
+    <row r="57" spans="1:27" ht="100.8">
+      <c r="A57" s="46"/>
       <c r="B57" s="3" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="E57" s="33" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="3"/>
@@ -3152,19 +3190,19 @@
       <c r="Z57" s="4"/>
       <c r="AA57" s="4"/>
     </row>
-    <row r="58" spans="1:27" ht="57.6">
-      <c r="A58" s="5"/>
+    <row r="58" spans="1:27" ht="42" customHeight="1">
+      <c r="A58" s="46"/>
       <c r="B58" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>148</v>
+      <c r="E58" s="33" t="s">
+        <v>173</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="3"/>
@@ -3189,21 +3227,19 @@
       <c r="Z58" s="4"/>
       <c r="AA58" s="4"/>
     </row>
-    <row r="59" spans="1:27" ht="28.8">
-      <c r="A59" s="5" t="s">
-        <v>66</v>
+    <row r="59" spans="1:27" ht="43.2">
+      <c r="A59" s="46"/>
+      <c r="B59" s="3" t="s">
+        <v>147</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C59" s="14" t="s">
-        <v>146</v>
+      <c r="C59" s="15" t="s">
+        <v>174</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
-      <c r="E59" s="3" t="s">
-        <v>80</v>
+      <c r="E59" s="33" t="s">
+        <v>161</v>
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="3"/>
@@ -3228,19 +3264,19 @@
       <c r="Z59" s="4"/>
       <c r="AA59" s="4"/>
     </row>
-    <row r="60" spans="1:27" ht="27.6">
-      <c r="A60" s="5"/>
+    <row r="60" spans="1:27" ht="57.6">
+      <c r="A60" s="46"/>
       <c r="B60" s="3" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
-      <c r="C60" s="44" t="s">
-        <v>149</v>
+      <c r="C60" s="15" t="s">
+        <v>164</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>153</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>80</v>
+        <v>167</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="3"/>
@@ -3265,22 +3301,21 @@
       <c r="Z60" s="4"/>
       <c r="AA60" s="4"/>
     </row>
-    <row r="61" spans="1:27" ht="41.4">
-      <c r="A61" s="5"/>
+    <row r="61" spans="1:27" ht="28.8">
+      <c r="A61" s="46"/>
       <c r="B61" s="3" t="s">
-        <v>151</v>
+        <v>106</v>
       </c>
-      <c r="C61" s="44" t="s">
-        <v>169</v>
+      <c r="C61" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>152</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>150</v>
+        <v>79</v>
       </c>
       <c r="F61" s="4"/>
-      <c r="G61" s="3"/>
       <c r="H61" s="15"/>
       <c r="I61" s="3"/>
       <c r="J61" s="4"/>
@@ -3302,19 +3337,19 @@
       <c r="Z61" s="4"/>
       <c r="AA61" s="4"/>
     </row>
-    <row r="62" spans="1:27" ht="41.4">
-      <c r="A62" s="5"/>
+    <row r="62" spans="1:27" ht="27.6">
+      <c r="A62" s="46"/>
       <c r="B62" s="3" t="s">
-        <v>166</v>
+        <v>107</v>
       </c>
-      <c r="C62" s="45" t="s">
-        <v>170</v>
+      <c r="C62" s="44" t="s">
+        <v>148</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>152</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>150</v>
+        <v>79</v>
       </c>
       <c r="F62" s="4"/>
       <c r="G62" s="3"/>
@@ -3339,12 +3374,20 @@
       <c r="Z62" s="4"/>
       <c r="AA62" s="4"/>
     </row>
-    <row r="63" spans="1:27" ht="14.4">
-      <c r="A63" s="5"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="44"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
+    <row r="63" spans="1:27" ht="41.4">
+      <c r="A63" s="46"/>
+      <c r="B63" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C63" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>149</v>
+      </c>
       <c r="F63" s="4"/>
       <c r="G63" s="3"/>
       <c r="H63" s="15"/>
@@ -3368,12 +3411,24 @@
       <c r="Z63" s="4"/>
       <c r="AA63" s="4"/>
     </row>
-    <row r="64" spans="1:27" ht="14.4">
-      <c r="A64" s="5"/>
+    <row r="64" spans="1:27" ht="41.4">
+      <c r="A64" s="46"/>
+      <c r="B64" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C64" s="45" t="s">
+        <v>166</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>149</v>
+      </c>
       <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="6"/>
-      <c r="I64" s="4"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="3"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
@@ -3393,11 +3448,23 @@
       <c r="Z64" s="4"/>
       <c r="AA64" s="4"/>
     </row>
-    <row r="65" spans="1:27" ht="14.4">
-      <c r="A65" s="5"/>
+    <row r="65" spans="1:27" ht="78">
+      <c r="A65" s="46"/>
+      <c r="B65" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C65" s="49" t="s">
+        <v>178</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>147</v>
+      </c>
       <c r="F65" s="4"/>
       <c r="G65" s="3"/>
-      <c r="H65" s="6"/>
+      <c r="H65" s="15"/>
       <c r="I65" s="3"/>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
@@ -3419,11 +3486,7 @@
       <c r="AA65" s="4"/>
     </row>
     <row r="66" spans="1:27" ht="14.4">
-      <c r="A66" s="5"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="6"/>
+      <c r="A66" s="46"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
       <c r="H66" s="6"/>
@@ -3448,15 +3511,11 @@
       <c r="AA66" s="4"/>
     </row>
     <row r="67" spans="1:27" ht="14.4">
-      <c r="A67" s="6"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="6"/>
+      <c r="A67" s="46"/>
       <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
+      <c r="G67" s="3"/>
       <c r="H67" s="6"/>
-      <c r="I67" s="4"/>
+      <c r="I67" s="3"/>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
@@ -3477,7 +3536,7 @@
       <c r="AA67" s="4"/>
     </row>
     <row r="68" spans="1:27" ht="14.4">
-      <c r="A68" s="6"/>
+      <c r="A68" s="46"/>
       <c r="B68" s="3"/>
       <c r="C68" s="15"/>
       <c r="D68" s="4"/>
@@ -3506,7 +3565,7 @@
       <c r="AA68" s="4"/>
     </row>
     <row r="69" spans="1:27" ht="14.4">
-      <c r="A69" s="6"/>
+      <c r="A69" s="48"/>
       <c r="B69" s="3"/>
       <c r="C69" s="15"/>
       <c r="D69" s="4"/>
@@ -3535,7 +3594,7 @@
       <c r="AA69" s="4"/>
     </row>
     <row r="70" spans="1:27" ht="14.4">
-      <c r="A70" s="6"/>
+      <c r="A70" s="48"/>
       <c r="B70" s="3"/>
       <c r="C70" s="15"/>
       <c r="D70" s="4"/>
@@ -31780,8 +31839,66 @@
       <c r="Z1043" s="4"/>
       <c r="AA1043" s="4"/>
     </row>
-    <row r="1044" spans="1:27" ht="15.75" customHeight="1">
+    <row r="1044" spans="1:27" ht="14.4">
       <c r="A1044" s="6"/>
+      <c r="B1044" s="3"/>
+      <c r="C1044" s="15"/>
+      <c r="D1044" s="4"/>
+      <c r="E1044" s="6"/>
+      <c r="F1044" s="4"/>
+      <c r="G1044" s="4"/>
+      <c r="H1044" s="6"/>
+      <c r="I1044" s="4"/>
+      <c r="J1044" s="4"/>
+      <c r="K1044" s="4"/>
+      <c r="L1044" s="4"/>
+      <c r="M1044" s="4"/>
+      <c r="N1044" s="4"/>
+      <c r="O1044" s="4"/>
+      <c r="P1044" s="4"/>
+      <c r="Q1044" s="4"/>
+      <c r="R1044" s="4"/>
+      <c r="S1044" s="4"/>
+      <c r="T1044" s="4"/>
+      <c r="U1044" s="4"/>
+      <c r="V1044" s="4"/>
+      <c r="W1044" s="4"/>
+      <c r="X1044" s="4"/>
+      <c r="Y1044" s="4"/>
+      <c r="Z1044" s="4"/>
+      <c r="AA1044" s="4"/>
+    </row>
+    <row r="1045" spans="1:27" ht="14.4">
+      <c r="A1045" s="6"/>
+      <c r="B1045" s="3"/>
+      <c r="C1045" s="15"/>
+      <c r="D1045" s="4"/>
+      <c r="E1045" s="6"/>
+      <c r="F1045" s="4"/>
+      <c r="G1045" s="4"/>
+      <c r="H1045" s="6"/>
+      <c r="I1045" s="4"/>
+      <c r="J1045" s="4"/>
+      <c r="K1045" s="4"/>
+      <c r="L1045" s="4"/>
+      <c r="M1045" s="4"/>
+      <c r="N1045" s="4"/>
+      <c r="O1045" s="4"/>
+      <c r="P1045" s="4"/>
+      <c r="Q1045" s="4"/>
+      <c r="R1045" s="4"/>
+      <c r="S1045" s="4"/>
+      <c r="T1045" s="4"/>
+      <c r="U1045" s="4"/>
+      <c r="V1045" s="4"/>
+      <c r="W1045" s="4"/>
+      <c r="X1045" s="4"/>
+      <c r="Y1045" s="4"/>
+      <c r="Z1045" s="4"/>
+      <c r="AA1045" s="4"/>
+    </row>
+    <row r="1046" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A1046" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated codebboks to reflect changes of  template 1,2,3 of shell tables for SAP v2.3
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\DP3-MS-SLE\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\DP3-MS-SLE - Copy\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74299BE3-AF74-41BF-A88C-A121147B298E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CC1AA6-1B5D-44EB-9006-7E4FBE056CA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="9045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -536,9 +536,6 @@
     <t>D3_DU_PREGNANCY_COHORT_variables</t>
   </si>
   <si>
-    <t>D3_DU_PREGNANCY_COHORT_variables D4_DU_MS_COHORT</t>
-  </si>
-  <si>
     <t>D4_DU_matched_MS_PREGNANCY_COHORT_to_MS_COHORT</t>
   </si>
   <si>
@@ -558,6 +555,9 @@
   </si>
   <si>
     <t>D4_DU_PREGNANCY_COHORT D3_SAP1_MS_COHORT D3_study_population_SAP1</t>
+  </si>
+  <si>
+    <t>D3_DU_PREGNANCY_COHORT_variables D4_DU_MS_COHORT D3_DU_selection_criteria_from_pregnancies_to_DU_PREGNANCY-COHORT</t>
   </si>
 </sst>
 </file>
@@ -1015,11 +1015,11 @@
   </sheetPr>
   <dimension ref="A1:AA1046"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E41" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E49" sqref="E49"/>
+      <selection pane="bottomRight" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -2862,7 +2862,7 @@
         <v>132</v>
       </c>
       <c r="E49" s="32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F49" s="34"/>
       <c r="G49" s="4"/>
@@ -2975,7 +2975,7 @@
         <v>146</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="F52" s="34"/>
       <c r="G52" s="4"/>
@@ -3003,7 +3003,7 @@
     <row r="53" spans="1:27" ht="90">
       <c r="A53" s="45"/>
       <c r="B53" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C53" s="15" t="s">
         <v>78</v>
@@ -3012,7 +3012,7 @@
         <v>145</v>
       </c>
       <c r="E53" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F53" s="34"/>
       <c r="G53" s="4"/>
@@ -3049,7 +3049,7 @@
         <v>145</v>
       </c>
       <c r="E54" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F54" s="34"/>
       <c r="G54" s="4"/>
@@ -3113,7 +3113,7 @@
       <c r="Z55" s="4"/>
       <c r="AA55" s="4"/>
     </row>
-    <row r="56" spans="1:27" ht="94.5">
+    <row r="56" spans="1:27" ht="30" customHeight="1">
       <c r="A56" s="45"/>
       <c r="B56" s="3" t="s">
         <v>156</v>
@@ -3125,7 +3125,7 @@
         <v>155</v>
       </c>
       <c r="E56" s="33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="3"/>
@@ -3150,7 +3150,7 @@
       <c r="Z56" s="4"/>
       <c r="AA56" s="4"/>
     </row>
-    <row r="57" spans="1:27" ht="105">
+    <row r="57" spans="1:27" ht="28.5" customHeight="1">
       <c r="A57" s="45"/>
       <c r="B57" s="3" t="s">
         <v>154</v>
@@ -3162,7 +3162,7 @@
         <v>155</v>
       </c>
       <c r="E57" s="33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="3"/>
@@ -3199,7 +3199,7 @@
         <v>158</v>
       </c>
       <c r="E58" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="3"/>
@@ -3236,7 +3236,7 @@
         <v>157</v>
       </c>
       <c r="E59" s="33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="3"/>
@@ -3448,7 +3448,7 @@
     <row r="65" spans="1:27" ht="78.75">
       <c r="A65" s="45"/>
       <c r="B65" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C65" s="48" t="s">
         <v>162</v>

</xml_diff>

<commit_message>
Updated codebooks and index
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\DP3-MS-SLE - Copy\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9E89FF-8EAA-40B4-AAD9-2EAEFBE7FFA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9734A338-82A7-4EA4-9727-82C49CDE5921}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="9045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -557,13 +557,13 @@
     <t>D4_DU_PREGNANCY_COHORT D3_SAP1_MS_COHORT D3_study_population_SAP1</t>
   </si>
   <si>
-    <t>D3_DU_PREGNANCY_COHORT_variables D4_DU_MS_COHORT D3_DU_selection_criteria_from_pregnancies_to_DU_PREGNANCY-COHORT</t>
-  </si>
-  <si>
     <t>10_T3_21_aggregate_prevalence_of_exclusive_use_MSmeds_in_MSpregnancy_trimesters</t>
   </si>
   <si>
     <t>D4_DU_individual_prevalence_of_use_MSmeds_in_MSpregnancy_trimesters conceptsetdataset</t>
+  </si>
+  <si>
+    <t>D4_DU_MS_COHORT D3_DU_selection_criteria_from_pregnancies_to_DU_PREGNANCY-COHORT</t>
   </si>
 </sst>
 </file>
@@ -1021,19 +1021,19 @@
   </sheetPr>
   <dimension ref="A1:AA1046"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E51" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E52" sqref="E52"/>
+      <selection pane="bottomRight" activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="64.85546875" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" style="40" customWidth="1"/>
-    <col min="4" max="4" width="48.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="40" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="46" customWidth="1"/>
     <col min="7" max="7" width="28.28515625" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" customWidth="1"/>
@@ -2614,7 +2614,7 @@
       <c r="Z41" s="4"/>
       <c r="AA41" s="4"/>
     </row>
-    <row r="42" spans="1:27" ht="45">
+    <row r="42" spans="1:27" ht="60">
       <c r="A42" s="45"/>
       <c r="B42" s="25" t="s">
         <v>164</v>
@@ -2651,7 +2651,7 @@
       <c r="Z42" s="4"/>
       <c r="AA42" s="4"/>
     </row>
-    <row r="43" spans="1:27" ht="45">
+    <row r="43" spans="1:27" ht="90">
       <c r="A43" s="45"/>
       <c r="B43" s="32" t="s">
         <v>68</v>
@@ -2690,7 +2690,7 @@
       <c r="Z43" s="4"/>
       <c r="AA43" s="4"/>
     </row>
-    <row r="44" spans="1:27" ht="60">
+    <row r="44" spans="1:27" ht="90">
       <c r="A44" s="45"/>
       <c r="B44" s="32" t="s">
         <v>165</v>
@@ -2729,7 +2729,7 @@
       <c r="Z44" s="4"/>
       <c r="AA44" s="4"/>
     </row>
-    <row r="45" spans="1:27" ht="30">
+    <row r="45" spans="1:27" ht="45">
       <c r="A45" s="45"/>
       <c r="B45" s="32" t="s">
         <v>166</v>
@@ -2768,7 +2768,7 @@
       <c r="Z45" s="4"/>
       <c r="AA45" s="4"/>
     </row>
-    <row r="46" spans="1:27" ht="30">
+    <row r="46" spans="1:27" ht="45">
       <c r="A46" s="45"/>
       <c r="B46" s="33" t="s">
         <v>72</v>
@@ -2819,7 +2819,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="30">
+    <row r="48" spans="1:27" ht="45">
       <c r="A48" s="45"/>
       <c r="B48" s="3" t="s">
         <v>169</v>
@@ -2856,7 +2856,7 @@
       <c r="Z48" s="4"/>
       <c r="AA48" s="4"/>
     </row>
-    <row r="49" spans="1:27" ht="26.25">
+    <row r="49" spans="1:27" ht="39">
       <c r="A49" s="45"/>
       <c r="B49" s="33" t="s">
         <v>170</v>
@@ -2895,7 +2895,7 @@
       <c r="Z49" s="4"/>
       <c r="AA49" s="4"/>
     </row>
-    <row r="50" spans="1:27" ht="60">
+    <row r="50" spans="1:27" ht="90">
       <c r="A50" s="45"/>
       <c r="B50" s="33" t="s">
         <v>100</v>
@@ -2932,7 +2932,7 @@
       <c r="Z50" s="4"/>
       <c r="AA50" s="4"/>
     </row>
-    <row r="51" spans="1:27" ht="75">
+    <row r="51" spans="1:27" ht="120">
       <c r="A51" s="45"/>
       <c r="B51" s="33" t="s">
         <v>101</v>
@@ -2969,7 +2969,7 @@
       <c r="Z51" s="4"/>
       <c r="AA51" s="4"/>
     </row>
-    <row r="52" spans="1:27" ht="60">
+    <row r="52" spans="1:27" ht="90">
       <c r="A52" s="45"/>
       <c r="B52" s="3" t="s">
         <v>148</v>
@@ -2981,7 +2981,7 @@
         <v>146</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F52" s="34"/>
       <c r="G52" s="4"/>
@@ -3006,7 +3006,7 @@
       <c r="Z52" s="4"/>
       <c r="AA52" s="4"/>
     </row>
-    <row r="53" spans="1:27" ht="90">
+    <row r="53" spans="1:27" ht="150">
       <c r="A53" s="45"/>
       <c r="B53" s="3" t="s">
         <v>171</v>
@@ -3043,7 +3043,7 @@
       <c r="Z53" s="4"/>
       <c r="AA53" s="4"/>
     </row>
-    <row r="54" spans="1:27" ht="60">
+    <row r="54" spans="1:27" ht="105">
       <c r="A54" s="45"/>
       <c r="B54" s="3" t="s">
         <v>97</v>
@@ -3080,7 +3080,7 @@
       <c r="Z54" s="4"/>
       <c r="AA54" s="4"/>
     </row>
-    <row r="55" spans="1:27" ht="60">
+    <row r="55" spans="1:27" ht="105">
       <c r="A55" s="45"/>
       <c r="B55" s="3" t="s">
         <v>77</v>
@@ -3165,10 +3165,10 @@
         <v>160</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E57" s="33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="3"/>
@@ -3230,7 +3230,7 @@
       <c r="Z58" s="4"/>
       <c r="AA58" s="4"/>
     </row>
-    <row r="59" spans="1:27" ht="45">
+    <row r="59" spans="1:27" ht="75">
       <c r="A59" s="45"/>
       <c r="B59" s="3" t="s">
         <v>137</v>
@@ -3267,7 +3267,7 @@
       <c r="Z59" s="4"/>
       <c r="AA59" s="4"/>
     </row>
-    <row r="60" spans="1:27" ht="60">
+    <row r="60" spans="1:27" ht="90">
       <c r="A60" s="45"/>
       <c r="B60" s="3" t="s">
         <v>136</v>
@@ -3304,7 +3304,7 @@
       <c r="Z60" s="4"/>
       <c r="AA60" s="4"/>
     </row>
-    <row r="61" spans="1:27" ht="45">
+    <row r="61" spans="1:27" ht="60">
       <c r="A61" s="45"/>
       <c r="B61" s="3" t="s">
         <v>102</v>
@@ -3340,7 +3340,7 @@
       <c r="Z61" s="4"/>
       <c r="AA61" s="4"/>
     </row>
-    <row r="62" spans="1:27" ht="26.25">
+    <row r="62" spans="1:27" ht="39">
       <c r="A62" s="45"/>
       <c r="B62" s="3" t="s">
         <v>103</v>
@@ -3377,7 +3377,7 @@
       <c r="Z62" s="4"/>
       <c r="AA62" s="4"/>
     </row>
-    <row r="63" spans="1:27" ht="39">
+    <row r="63" spans="1:27" ht="51.75">
       <c r="A63" s="45"/>
       <c r="B63" s="3" t="s">
         <v>140</v>
@@ -3414,7 +3414,7 @@
       <c r="Z63" s="4"/>
       <c r="AA63" s="4"/>
     </row>
-    <row r="64" spans="1:27" ht="38.25">
+    <row r="64" spans="1:27" ht="51">
       <c r="A64" s="45"/>
       <c r="B64" s="3" t="s">
         <v>150</v>
@@ -3451,7 +3451,7 @@
       <c r="Z64" s="4"/>
       <c r="AA64" s="4"/>
     </row>
-    <row r="65" spans="1:27" ht="78.75">
+    <row r="65" spans="1:27" ht="141.75">
       <c r="A65" s="45"/>
       <c r="B65" s="3" t="s">
         <v>172</v>

</xml_diff>